<commit_message>
updating dates from storm2 2023 water samples
</commit_message>
<xml_diff>
--- a/GSD/Water Samples/LaJara_LISST_GSD_Summer2023.xlsx
+++ b/GSD/Water Samples/LaJara_LISST_GSD_Summer2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vandalsuidaho-my.sharepoint.com/personal/huck4481_vandals_uidaho_edu/Documents/Desktop/Research/La Jara Data/Fine GSD/Water Samples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Water Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="864" documentId="13_ncr:1_{39D493F6-EBF7-4392-B921-C253990D5D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FFD0F7F-3D89-40F3-9305-7CD68D5235C0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FA37B6-0301-4AF9-9ED3-CD6BE2A29EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="4" xr2:uid="{5952B5DA-6B13-43D1-9193-1BE03F62DE4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5952B5DA-6B13-43D1-9193-1BE03F62DE4B}"/>
   </bookViews>
   <sheets>
     <sheet name="&quot;Storm&quot; 1" sheetId="2" r:id="rId1"/>
@@ -1543,7 +1543,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1903,25 +1903,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1967,8 +1955,20 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2286,8 +2286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CFA7B-6AB5-4D15-9587-78BC8AED2040}">
   <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O118" sqref="O117:O118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2306,10 +2306,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>17</v>
       </c>
       <c r="B112" s="14">
-        <v>45136</v>
+        <v>45136.629861111112</v>
       </c>
       <c r="C112" s="4">
         <v>1</v>
@@ -4888,7 +4888,7 @@
       <c r="G112" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="H112" s="32" t="s">
+      <c r="H112" s="51" t="s">
         <v>238</v>
       </c>
       <c r="I112" s="20" t="s">
@@ -4906,7 +4906,7 @@
         <v>17</v>
       </c>
       <c r="B113" s="14">
-        <v>45136</v>
+        <v>45136.629861111112</v>
       </c>
       <c r="C113" s="4">
         <v>0</v>
@@ -4923,7 +4923,7 @@
       <c r="G113" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="H113" s="33"/>
+      <c r="H113" s="52"/>
       <c r="I113" s="23" t="s">
         <v>202</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>17</v>
       </c>
       <c r="B114" s="14">
-        <v>45136</v>
+        <v>45136.629861111112</v>
       </c>
       <c r="C114" s="4">
         <v>1</v>
@@ -4959,7 +4959,7 @@
         <v>17</v>
       </c>
       <c r="B115" s="14">
-        <v>45136</v>
+        <v>45136.629861111112</v>
       </c>
       <c r="C115" s="4">
         <v>1</v>
@@ -4982,7 +4982,7 @@
         <v>17</v>
       </c>
       <c r="B116" s="14">
-        <v>45136</v>
+        <v>45136.629861111112</v>
       </c>
       <c r="C116" s="4">
         <v>1</v>
@@ -5005,7 +5005,7 @@
         <v>18</v>
       </c>
       <c r="B117" s="14">
-        <v>45136</v>
+        <v>45136.640277777777</v>
       </c>
       <c r="C117" s="4">
         <v>0</v>
@@ -5022,7 +5022,7 @@
       <c r="G117" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="H117" s="32" t="s">
+      <c r="H117" s="51" t="s">
         <v>206</v>
       </c>
       <c r="I117" s="20" t="s">
@@ -5040,7 +5040,7 @@
         <v>18</v>
       </c>
       <c r="B118" s="14">
-        <v>45136</v>
+        <v>45136.640277777777</v>
       </c>
       <c r="C118" s="4">
         <v>1</v>
@@ -5057,7 +5057,7 @@
       <c r="G118" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="H118" s="33"/>
+      <c r="H118" s="52"/>
       <c r="I118" s="23" t="s">
         <v>202</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>18</v>
       </c>
       <c r="B119" s="14">
-        <v>45136</v>
+        <v>45136.640277777777</v>
       </c>
       <c r="C119" s="4">
         <v>1</v>
@@ -5093,7 +5093,7 @@
         <v>18</v>
       </c>
       <c r="B120" s="14">
-        <v>45136</v>
+        <v>45136.640277777777</v>
       </c>
       <c r="C120" s="4">
         <v>1</v>
@@ -5116,7 +5116,7 @@
         <v>18</v>
       </c>
       <c r="B121" s="14">
-        <v>45136</v>
+        <v>45136.640277777777</v>
       </c>
       <c r="C121" s="4">
         <v>1</v>
@@ -5139,7 +5139,7 @@
         <v>18</v>
       </c>
       <c r="B122" s="14">
-        <v>45136</v>
+        <v>45136.640277777777</v>
       </c>
       <c r="C122" s="4">
         <v>1</v>
@@ -5162,7 +5162,7 @@
         <v>19</v>
       </c>
       <c r="B123" s="14">
-        <v>45136</v>
+        <v>45136.650694444441</v>
       </c>
       <c r="C123" s="4">
         <v>0</v>
@@ -5185,7 +5185,7 @@
         <v>19</v>
       </c>
       <c r="B124" s="14">
-        <v>45136</v>
+        <v>45136.650694444441</v>
       </c>
       <c r="C124" s="4">
         <v>0</v>
@@ -5208,7 +5208,7 @@
         <v>19</v>
       </c>
       <c r="B125" s="14">
-        <v>45136</v>
+        <v>45136.650694444441</v>
       </c>
       <c r="C125" s="4">
         <v>0</v>
@@ -5231,7 +5231,7 @@
         <v>19</v>
       </c>
       <c r="B126" s="14">
-        <v>45136</v>
+        <v>45136.650694444441</v>
       </c>
       <c r="C126" s="4">
         <v>1</v>
@@ -5248,7 +5248,7 @@
       <c r="G126" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="H126" s="32" t="s">
+      <c r="H126" s="51" t="s">
         <v>250</v>
       </c>
       <c r="I126" s="20" t="s">
@@ -5263,7 +5263,7 @@
         <v>20</v>
       </c>
       <c r="B127" s="14">
-        <v>45136</v>
+        <v>45136.661111111112</v>
       </c>
       <c r="C127" s="4">
         <v>0</v>
@@ -5280,7 +5280,7 @@
       <c r="G127" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="H127" s="33"/>
+      <c r="H127" s="52"/>
       <c r="I127" s="23" t="s">
         <v>202</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>20</v>
       </c>
       <c r="B128" s="14">
-        <v>45136</v>
+        <v>45136.661111111112</v>
       </c>
       <c r="C128" s="4">
         <v>0</v>
@@ -5316,7 +5316,7 @@
         <v>20</v>
       </c>
       <c r="B129" s="14">
-        <v>45136</v>
+        <v>45136.661111111112</v>
       </c>
       <c r="C129" s="4">
         <v>0</v>
@@ -5339,7 +5339,7 @@
         <v>20</v>
       </c>
       <c r="B130" s="14">
-        <v>45136</v>
+        <v>45136.661111111112</v>
       </c>
       <c r="C130" s="4">
         <v>0</v>
@@ -5362,7 +5362,7 @@
         <v>21</v>
       </c>
       <c r="B131" s="14">
-        <v>45136</v>
+        <v>45136.671527777777</v>
       </c>
       <c r="C131" s="4">
         <v>0</v>
@@ -5385,7 +5385,7 @@
         <v>21</v>
       </c>
       <c r="B132" s="14">
-        <v>45136</v>
+        <v>45136.671527777777</v>
       </c>
       <c r="C132" s="4">
         <v>0</v>
@@ -5408,7 +5408,7 @@
         <v>21</v>
       </c>
       <c r="B133" s="14">
-        <v>45136</v>
+        <v>45136.671527777777</v>
       </c>
       <c r="C133" s="4">
         <v>0</v>
@@ -5431,7 +5431,7 @@
         <v>21</v>
       </c>
       <c r="B134" s="14">
-        <v>45136</v>
+        <v>45136.671527777777</v>
       </c>
       <c r="C134" s="4">
         <v>0</v>
@@ -5454,7 +5454,7 @@
         <v>21</v>
       </c>
       <c r="B135" s="14">
-        <v>45136</v>
+        <v>45136.671527777777</v>
       </c>
       <c r="C135" s="4">
         <v>0</v>
@@ -5487,8 +5487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEA57E8-AC6C-4413-9DB1-76B8A0DB268F}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5504,10 +5504,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -6034,7 +6034,9 @@
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="9">
+        <v>45151.78125</v>
+      </c>
       <c r="C26" s="4">
         <v>0</v>
       </c>
@@ -6055,7 +6057,9 @@
       <c r="A27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="9">
+        <v>45151.78125</v>
+      </c>
       <c r="C27" s="4">
         <v>0</v>
       </c>
@@ -6076,7 +6080,9 @@
       <c r="A28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="9">
+        <v>45151.78125</v>
+      </c>
       <c r="C28" s="4">
         <v>0</v>
       </c>
@@ -6097,7 +6103,9 @@
       <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="9">
+        <v>45151.78125</v>
+      </c>
       <c r="C29" s="4">
         <v>0</v>
       </c>
@@ -6118,7 +6126,9 @@
       <c r="A30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="9">
+        <v>45151.78125</v>
+      </c>
       <c r="C30" s="4">
         <v>0</v>
       </c>
@@ -6139,7 +6149,9 @@
       <c r="A31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="9">
+        <v>45151.791666666664</v>
+      </c>
       <c r="C31" s="4">
         <v>0</v>
       </c>
@@ -6160,7 +6172,9 @@
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="4"/>
+      <c r="B32" s="9">
+        <v>45151.791666666664</v>
+      </c>
       <c r="C32" s="4">
         <v>0</v>
       </c>
@@ -6181,7 +6195,9 @@
       <c r="A33" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="4"/>
+      <c r="B33" s="9">
+        <v>45151.791666666664</v>
+      </c>
       <c r="C33" s="4">
         <v>0</v>
       </c>
@@ -6202,7 +6218,9 @@
       <c r="A34" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="9">
+        <v>45151.791666666664</v>
+      </c>
       <c r="C34" s="4">
         <v>0</v>
       </c>
@@ -6223,7 +6241,9 @@
       <c r="A35" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="4"/>
+      <c r="B35" s="9">
+        <v>45151.791666666664</v>
+      </c>
       <c r="C35" s="4">
         <v>0</v>
       </c>
@@ -6244,7 +6264,9 @@
       <c r="A36" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="4"/>
+      <c r="B36" s="9">
+        <v>45151.802083333336</v>
+      </c>
       <c r="C36" s="4">
         <v>0</v>
       </c>
@@ -6265,7 +6287,9 @@
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="4"/>
+      <c r="B37" s="9">
+        <v>45151.802083333336</v>
+      </c>
       <c r="C37" s="4">
         <v>0</v>
       </c>
@@ -6286,7 +6310,9 @@
       <c r="A38" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="9">
+        <v>45151.802083333336</v>
+      </c>
       <c r="C38" s="4">
         <v>0</v>
       </c>
@@ -6307,7 +6333,9 @@
       <c r="A39" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="4"/>
+      <c r="B39" s="9">
+        <v>45151.802083333336</v>
+      </c>
       <c r="C39" s="4">
         <v>0</v>
       </c>
@@ -6328,7 +6356,9 @@
       <c r="A40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="9">
+        <v>45151.8125</v>
+      </c>
       <c r="C40" s="4">
         <v>0</v>
       </c>
@@ -6349,7 +6379,9 @@
       <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="9">
+        <v>45151.8125</v>
+      </c>
       <c r="C41" s="4">
         <v>0</v>
       </c>
@@ -6370,7 +6402,9 @@
       <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="9">
+        <v>45151.8125</v>
+      </c>
       <c r="C42" s="4">
         <v>0</v>
       </c>
@@ -6391,7 +6425,9 @@
       <c r="A43" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="4"/>
+      <c r="B43" s="9">
+        <v>45151.8125</v>
+      </c>
       <c r="C43" s="4">
         <v>0</v>
       </c>
@@ -6408,7 +6444,9 @@
       <c r="A44" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="4"/>
+      <c r="B44" s="9">
+        <v>45151.822916666664</v>
+      </c>
       <c r="C44" s="4">
         <v>0</v>
       </c>
@@ -6429,7 +6467,9 @@
       <c r="A45" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B45" s="4"/>
+      <c r="B45" s="9">
+        <v>45151.833333333336</v>
+      </c>
       <c r="C45" s="4">
         <v>0</v>
       </c>
@@ -6450,7 +6490,9 @@
       <c r="A46" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="4"/>
+      <c r="B46" s="9">
+        <v>45151.84375</v>
+      </c>
       <c r="C46" s="4">
         <v>0</v>
       </c>
@@ -6471,7 +6513,9 @@
       <c r="A47" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="4"/>
+      <c r="B47" s="9">
+        <v>45151.854166666664</v>
+      </c>
       <c r="C47" s="4">
         <v>0</v>
       </c>
@@ -6492,7 +6536,9 @@
       <c r="A48" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="4"/>
+      <c r="B48" s="9">
+        <v>45151.864583333336</v>
+      </c>
       <c r="C48" s="4">
         <v>0</v>
       </c>
@@ -6513,7 +6559,9 @@
       <c r="A49" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="4"/>
+      <c r="B49" s="9">
+        <v>45151.864583333336</v>
+      </c>
       <c r="C49" s="4">
         <v>0</v>
       </c>
@@ -6534,7 +6582,9 @@
       <c r="A50" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B50" s="4"/>
+      <c r="B50" s="9">
+        <v>45151.864583333336</v>
+      </c>
       <c r="C50" s="4">
         <v>0</v>
       </c>
@@ -6555,7 +6605,9 @@
       <c r="A51" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="4"/>
+      <c r="B51" s="9">
+        <v>45151.864583333336</v>
+      </c>
       <c r="C51" s="4">
         <v>0</v>
       </c>
@@ -6576,7 +6628,9 @@
       <c r="A52" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="4"/>
+      <c r="B52" s="9">
+        <v>45151.864583333336</v>
+      </c>
       <c r="C52" s="4">
         <v>0</v>
       </c>
@@ -6597,7 +6651,9 @@
       <c r="A53" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B53" s="4"/>
+      <c r="B53" s="9">
+        <v>45151.875</v>
+      </c>
       <c r="C53" s="4">
         <v>0</v>
       </c>
@@ -6618,7 +6674,9 @@
       <c r="A54" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B54" s="4"/>
+      <c r="B54" s="9">
+        <v>45151.875</v>
+      </c>
       <c r="C54" s="4">
         <v>0</v>
       </c>
@@ -6639,7 +6697,9 @@
       <c r="A55" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B55" s="4"/>
+      <c r="B55" s="9">
+        <v>45151.875</v>
+      </c>
       <c r="C55" s="4">
         <v>0</v>
       </c>
@@ -6660,7 +6720,9 @@
       <c r="A56" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B56" s="4"/>
+      <c r="B56" s="9">
+        <v>45151.875</v>
+      </c>
       <c r="C56" s="4">
         <v>0</v>
       </c>
@@ -6681,7 +6743,9 @@
       <c r="A57" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B57" s="4"/>
+      <c r="B57" s="9">
+        <v>45151.875</v>
+      </c>
       <c r="C57" s="4">
         <v>0</v>
       </c>
@@ -6702,7 +6766,9 @@
       <c r="A58" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B58" s="4"/>
+      <c r="B58" s="9">
+        <v>45151.885416666664</v>
+      </c>
       <c r="C58" s="4">
         <v>0</v>
       </c>
@@ -6723,7 +6789,9 @@
       <c r="A59" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B59" s="4"/>
+      <c r="B59" s="9">
+        <v>45151.885416666664</v>
+      </c>
       <c r="C59" s="4">
         <v>0</v>
       </c>
@@ -6744,7 +6812,9 @@
       <c r="A60" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B60" s="4"/>
+      <c r="B60" s="9">
+        <v>45151.885416666664</v>
+      </c>
       <c r="C60" s="4">
         <v>0</v>
       </c>
@@ -6765,7 +6835,9 @@
       <c r="A61" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="4"/>
+      <c r="B61" s="9">
+        <v>45151.885416666664</v>
+      </c>
       <c r="C61" s="4">
         <v>0</v>
       </c>
@@ -6786,7 +6858,9 @@
       <c r="A62" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B62" s="4"/>
+      <c r="B62" s="9">
+        <v>45151.885416666664</v>
+      </c>
       <c r="C62" s="4">
         <v>0</v>
       </c>
@@ -6807,7 +6881,9 @@
       <c r="A63" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B63" s="4"/>
+      <c r="B63" s="9">
+        <v>45151.895833333336</v>
+      </c>
       <c r="C63" s="4">
         <v>0</v>
       </c>
@@ -6828,7 +6904,9 @@
       <c r="A64" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B64" s="4"/>
+      <c r="B64" s="9">
+        <v>45151.895833333336</v>
+      </c>
       <c r="C64" s="4">
         <v>0</v>
       </c>
@@ -6849,7 +6927,9 @@
       <c r="A65" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B65" s="4"/>
+      <c r="B65" s="9">
+        <v>45151.895833333336</v>
+      </c>
       <c r="C65" s="4">
         <v>0</v>
       </c>
@@ -6870,7 +6950,9 @@
       <c r="A66" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B66" s="4"/>
+      <c r="B66" s="9">
+        <v>45151.895833333336</v>
+      </c>
       <c r="C66" s="4">
         <v>0</v>
       </c>
@@ -6891,7 +6973,9 @@
       <c r="A67" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B67" s="4"/>
+      <c r="B67" s="9">
+        <v>45151.895833333336</v>
+      </c>
       <c r="C67" s="4">
         <v>0</v>
       </c>
@@ -6920,7 +7004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA95C67-CE3C-4E97-BF30-FAEAA97B4B4A}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="117" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -6937,10 +7021,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -8167,7 +8251,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8182,10 +8266,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -8401,50 +8485,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD81FE8B-68DD-410E-8571-EE78EDCA3E1E}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="49" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="23" style="49" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="49" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="49" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="49" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="49" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="49" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="49"/>
+    <col min="1" max="1" width="17.5703125" style="45" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="45" customWidth="1"/>
+    <col min="3" max="3" width="23" style="45" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="45" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="45" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="45" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="45" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="45" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="45" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="42" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="41" t="s">
         <v>435</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="41" t="s">
         <v>436</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="41" t="s">
         <v>437</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="41" t="s">
         <v>452</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="41" t="s">
         <v>438</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="41" t="s">
         <v>439</v>
       </c>
     </row>
@@ -8455,7 +8539,7 @@
       <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="33">
         <f>AVERAGE(D2:F2)</f>
         <v>95.963333333333324</v>
       </c>
@@ -8468,13 +8552,13 @@
       <c r="F2" s="4">
         <v>95.95</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="31" t="s">
         <v>455</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="31" t="s">
         <v>456</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="31" t="s">
         <v>457</v>
       </c>
     </row>
@@ -8485,7 +8569,7 @@
       <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="33">
         <f t="shared" ref="C3:C10" si="0">AVERAGE(D3:F3)</f>
         <v>80.180000000000007</v>
       </c>
@@ -8498,24 +8582,24 @@
       <c r="F3" s="4">
         <v>81.680000000000007</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="31" t="s">
         <v>458</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="31" t="s">
         <v>459</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="31" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="4" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="38" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="33">
         <f t="shared" si="0"/>
         <v>70.509999999999991</v>
       </c>
@@ -8525,7 +8609,7 @@
       <c r="E4" s="4">
         <v>71.44</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="36">
         <v>71.739999999999995</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -8539,13 +8623,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="38" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="33">
         <f t="shared" si="0"/>
         <v>48.22</v>
       </c>
@@ -8558,24 +8642,24 @@
       <c r="F5" s="4">
         <v>48.46</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="31" t="s">
         <v>462</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="31" t="s">
         <v>476</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="31" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="38" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="33">
         <f t="shared" si="0"/>
         <v>64.436666666666667</v>
       </c>
@@ -8599,13 +8683,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="38" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="33">
         <f t="shared" si="0"/>
         <v>48.583333333333336</v>
       </c>
@@ -8629,13 +8713,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="38" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="33">
         <f t="shared" si="0"/>
         <v>52.79999999999999</v>
       </c>
@@ -8645,7 +8729,7 @@
       <c r="E8" s="4">
         <v>51.91</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="36">
         <v>60.42</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -8659,13 +8743,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="38" t="s">
         <v>65</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="33">
         <f t="shared" si="0"/>
         <v>41.416666666666664</v>
       </c>
@@ -8689,46 +8773,46 @@
       </c>
     </row>
     <row r="10" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="38" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="33">
         <f t="shared" si="0"/>
         <v>39.299999999999997</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="31">
         <v>39.299999999999997</v>
       </c>
-      <c r="E10" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="35" t="s">
+      <c r="E10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="31" t="s">
         <v>467</v>
       </c>
-      <c r="H10" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I10" s="35" t="s">
+      <c r="H10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="31" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="49"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -8737,97 +8821,97 @@
       <c r="B12" s="4">
         <v>0</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="36">
         <f>AVERAGE(D12:F12)</f>
         <v>63.866666666666667</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="31">
         <v>63.92</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="31">
         <v>62.72</v>
       </c>
-      <c r="F12" s="35">
+      <c r="F12" s="31">
         <v>64.959999999999994</v>
       </c>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="31" t="s">
         <v>468</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="31" t="s">
         <v>486</v>
       </c>
-      <c r="I12" s="35" t="s">
+      <c r="I12" s="31" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="13" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="38" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="36">
         <f t="shared" ref="C13:C17" si="1">AVERAGE(D13:F13)</f>
         <v>75.403333333333322</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="31">
         <v>73.45</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="31">
         <v>74.239999999999995</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="31">
         <v>78.52</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="31" t="s">
         <v>469</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="31" t="s">
         <v>488</v>
       </c>
-      <c r="I13" s="35" t="s">
+      <c r="I13" s="31" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="14" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="38" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="4">
         <v>0</v>
       </c>
-      <c r="C14" s="40">
+      <c r="C14" s="36">
         <f t="shared" si="1"/>
         <v>70.74666666666667</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="31">
         <v>72.62</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="31">
         <v>66.72</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="31">
         <v>72.900000000000006</v>
       </c>
-      <c r="G14" s="35" t="s">
+      <c r="G14" s="31" t="s">
         <v>470</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="31" t="s">
         <v>490</v>
       </c>
-      <c r="I14" s="35" t="s">
+      <c r="I14" s="31" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="36">
         <f t="shared" si="1"/>
         <v>61.610000000000007</v>
       </c>
@@ -8851,13 +8935,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="38" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="4">
         <v>0</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="36">
         <f t="shared" si="1"/>
         <v>82.603333333333339</v>
       </c>
@@ -8887,578 +8971,578 @@
       <c r="B17" s="4">
         <v>0</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="36">
         <f t="shared" si="1"/>
         <v>54.116666666666667</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="31">
         <v>54.38</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="31">
         <v>52.57</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="31">
         <v>55.4</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="31" t="s">
         <v>473</v>
       </c>
-      <c r="H17" s="35" t="s">
+      <c r="H17" s="31" t="s">
         <v>496</v>
       </c>
-      <c r="I17" s="35" t="s">
+      <c r="I17" s="31" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="43"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="43"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="48"/>
-      <c r="I31" s="48"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="43"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="43"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="43"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="48"/>
+      <c r="A39" s="39"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
+      <c r="A43" s="46"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
+      <c r="A45" s="46"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
+      <c r="I46" s="39"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="51"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
+      <c r="A47" s="46"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="39"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="50"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="51"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
+      <c r="A48" s="46"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="51"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
+      <c r="A49" s="39"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="39"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="43"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48"/>
+      <c r="A50" s="39"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="43"/>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48"/>
+      <c r="A51" s="39"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="43"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="48"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="48"/>
+      <c r="A52" s="39"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="50"/>
-      <c r="B53" s="43"/>
-      <c r="C53" s="51"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="43"/>
+      <c r="A53" s="46"/>
+      <c r="B53" s="39"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="39"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="50"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="43"/>
-      <c r="I54" s="43"/>
+      <c r="A54" s="46"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="39"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="43"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43"/>
+      <c r="A55" s="39"/>
+      <c r="B55" s="39"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="43"/>
-      <c r="B56" s="43"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
+      <c r="A56" s="39"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="39"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="43"/>
-      <c r="B57" s="43"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="39"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="43"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="43"/>
-      <c r="E58" s="43"/>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="43"/>
-      <c r="I58" s="43"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="39"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="47"/>
-      <c r="B59" s="43"/>
-      <c r="C59" s="43"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="48"/>
+      <c r="A59" s="43"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="44"/>
+      <c r="I59" s="44"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="43"/>
-      <c r="B60" s="43"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="48"/>
-      <c r="H60" s="48"/>
-      <c r="I60" s="48"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="44"/>
+      <c r="I60" s="44"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="43"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="43"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="48"/>
+      <c r="A61" s="39"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="43"/>
-      <c r="B62" s="43"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="43"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="43"/>
-      <c r="G62" s="43"/>
-      <c r="H62" s="43"/>
-      <c r="I62" s="43"/>
+      <c r="A62" s="39"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="39"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="43"/>
-      <c r="B63" s="43"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
+      <c r="A63" s="39"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="39"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="43"/>
-      <c r="B64" s="43"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="43"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="43"/>
-      <c r="I64" s="43"/>
+      <c r="A64" s="39"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
+      <c r="I64" s="39"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="43"/>
-      <c r="B65" s="43"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="48"/>
-      <c r="H65" s="48"/>
-      <c r="I65" s="48"/>
+      <c r="A65" s="39"/>
+      <c r="B65" s="39"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="44"/>
+      <c r="I65" s="44"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="43"/>
-      <c r="B66" s="43"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="43"/>
-      <c r="H66" s="43"/>
-      <c r="I66" s="43"/>
+      <c r="A66" s="39"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="39"/>
+      <c r="I66" s="39"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="43"/>
-      <c r="B67" s="43"/>
-      <c r="C67" s="51"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
-      <c r="F67" s="43"/>
-      <c r="G67" s="43"/>
-      <c r="H67" s="43"/>
-      <c r="I67" s="43"/>
+      <c r="A67" s="39"/>
+      <c r="B67" s="39"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -9471,7 +9555,7 @@
   <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I67" sqref="A1:I67"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9479,9 +9563,9 @@
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="43"/>
-    <col min="6" max="6" width="9.5703125" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="43"/>
+    <col min="4" max="5" width="9.140625" style="39"/>
+    <col min="6" max="6" width="9.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="39"/>
     <col min="11" max="11" width="13.28515625" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" customWidth="1"/>
   </cols>
@@ -9496,22 +9580,22 @@
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="30" t="s">
         <v>435</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="30" t="s">
         <v>436</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="30" t="s">
         <v>437</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="30" t="s">
         <v>452</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="30" t="s">
         <v>438</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="30" t="s">
         <v>439</v>
       </c>
     </row>
@@ -9525,28 +9609,28 @@
       <c r="C2" s="18">
         <v>0</v>
       </c>
-      <c r="D2" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I2" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="39" t="s">
+      <c r="D2" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2" s="35" t="s">
         <v>319</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -9560,25 +9644,25 @@
       <c r="C3" s="18">
         <v>0</v>
       </c>
-      <c r="D3" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K3" s="38" t="s">
+      <c r="D3" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L3" s="4">
@@ -9592,7 +9676,7 @@
       <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="33">
         <f>AVERAGE(D4:F4)</f>
         <v>25.786666666666665</v>
       </c>
@@ -9614,7 +9698,7 @@
       <c r="I4" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L4" s="4">
@@ -9631,22 +9715,22 @@
       <c r="C5" s="18">
         <v>0</v>
       </c>
-      <c r="D5" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="35" t="s">
+      <c r="D5" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="31" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9679,15 +9763,15 @@
       <c r="I6" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="K6" s="35" t="s">
         <v>320</v>
       </c>
-      <c r="L6" s="39" t="s">
+      <c r="L6" s="35" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="37" t="s">
         <v>319</v>
       </c>
       <c r="B7" s="4">
@@ -9717,7 +9801,7 @@
       <c r="I7" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L7" s="4">
@@ -9725,7 +9809,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="37" t="s">
         <v>320</v>
       </c>
       <c r="B8" s="4">
@@ -9743,7 +9827,7 @@
         <f>138.03/(1-(L8/L7))</f>
         <v>230.05</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="36">
         <f>154.01/(1-(L8/L7))</f>
         <v>256.68333333333334</v>
       </c>
@@ -9756,7 +9840,7 @@
       <c r="I8" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L8" s="4">
@@ -9803,28 +9887,28 @@
       <c r="C10" s="18">
         <v>0</v>
       </c>
-      <c r="D10" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I10" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K10" s="39" t="s">
+      <c r="D10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K10" s="35" t="s">
         <v>327</v>
       </c>
-      <c r="L10" s="39" t="s">
+      <c r="L10" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -9838,25 +9922,25 @@
       <c r="C11" s="18">
         <v>0</v>
       </c>
-      <c r="D11" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K11" s="38" t="s">
+      <c r="D11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K11" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L11" s="4">
@@ -9873,25 +9957,25 @@
       <c r="C12" s="18">
         <v>0</v>
       </c>
-      <c r="D12" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I12" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K12" s="38" t="s">
+      <c r="D12" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L12" s="4">
@@ -9908,22 +9992,22 @@
       <c r="C13" s="18">
         <v>0</v>
       </c>
-      <c r="D13" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I13" s="35" t="s">
+      <c r="D13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="31" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9937,33 +10021,33 @@
       <c r="C14" s="18">
         <v>0</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I14" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K14" s="39" t="s">
+      <c r="D14" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14" s="35" t="s">
         <v>328</v>
       </c>
-      <c r="L14" s="39" t="s">
+      <c r="L14" s="35" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="37" t="s">
         <v>327</v>
       </c>
       <c r="B15" s="4">
@@ -9993,7 +10077,7 @@
       <c r="I15" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L15" s="4">
@@ -10001,13 +10085,13 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="37" t="s">
         <v>328</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="33">
         <f>AVERAGE(D16:F16)</f>
         <v>417.94666666666666</v>
       </c>
@@ -10032,7 +10116,7 @@
       <c r="I16" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="K16" s="38" t="s">
+      <c r="K16" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L16" s="4">
@@ -10049,33 +10133,33 @@
       <c r="C17" s="18">
         <v>0</v>
       </c>
-      <c r="D17" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F17" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I17" s="35" t="s">
+      <c r="D17" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="31" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="37" t="s">
         <v>333</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
       </c>
-      <c r="C18" s="37">
+      <c r="C18" s="33">
         <f>AVERAGE(D18:F18)</f>
         <v>279.34666666666664</v>
       </c>
@@ -10100,10 +10184,10 @@
       <c r="I18" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="K18" s="39" t="s">
+      <c r="K18" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="L18" s="39" t="s">
+      <c r="L18" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -10117,25 +10201,25 @@
       <c r="C19" s="18">
         <v>0</v>
       </c>
-      <c r="D19" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E19" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I19" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K19" s="38" t="s">
+      <c r="D19" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K19" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L19" s="4">
@@ -10152,25 +10236,25 @@
       <c r="C20" s="18">
         <v>0</v>
       </c>
-      <c r="D20" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G20" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K20" s="38" t="s">
+      <c r="D20" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K20" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L20" s="4">
@@ -10187,22 +10271,22 @@
       <c r="C21" s="18">
         <v>0</v>
       </c>
-      <c r="D21" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G21" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I21" s="35" t="s">
+      <c r="D21" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21" s="31" t="s">
         <v>99</v>
       </c>
     </row>
@@ -10216,51 +10300,51 @@
       <c r="C22" s="18">
         <v>0</v>
       </c>
-      <c r="D22" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H22" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I22" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" s="39" t="s">
+      <c r="D22" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I22" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K22" s="35" t="s">
         <v>339</v>
       </c>
-      <c r="L22" s="39" t="s">
+      <c r="L22" s="35" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="37" t="s">
         <v>339</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="33">
         <f>AVERAGE(D23:F23)</f>
         <v>360.625</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="36">
         <f>141.11/(1-(L24/L23))</f>
         <v>352.77500000000003</v>
       </c>
-      <c r="E23" s="40">
+      <c r="E23" s="36">
         <f>144.73/(1-(L24/L23))</f>
         <v>361.82499999999993</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="36">
         <f>146.91/(1-(L24/L23))</f>
         <v>367.27499999999998</v>
       </c>
@@ -10273,7 +10357,7 @@
       <c r="I23" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="K23" s="38" t="s">
+      <c r="K23" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L23" s="4">
@@ -10281,25 +10365,25 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="37" t="s">
         <v>340</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="33">
         <f t="shared" ref="C24:C28" si="0">AVERAGE(D24:F24)</f>
         <v>267.33333333333326</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="36">
         <f>107.02/(1-(L28/L27))</f>
         <v>267.54999999999995</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="36">
         <f>103.39/(1-(L28/L27))</f>
         <v>258.47499999999997</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F24" s="36">
         <f>110.39/(1-(L28/L27))</f>
         <v>275.97499999999997</v>
       </c>
@@ -10312,7 +10396,7 @@
       <c r="I24" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="K24" s="38" t="s">
+      <c r="K24" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L24" s="4">
@@ -10320,25 +10404,25 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="37" t="s">
         <v>341</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="33">
         <f t="shared" si="0"/>
         <v>139.08333333333334</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="36">
         <f>83.49/(1-(L32/L31))</f>
         <v>139.15</v>
       </c>
-      <c r="E25" s="40">
+      <c r="E25" s="36">
         <f>83.17/(1-(L32/L31))</f>
         <v>138.61666666666667</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="36">
         <f>83.69/(1-(L32/L31))</f>
         <v>139.48333333333335</v>
       </c>
@@ -10353,25 +10437,25 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="37" t="s">
         <v>342</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="33">
         <f t="shared" si="0"/>
         <v>133.66666666666666</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="36">
         <f>106.74/(1-(L36/L35))</f>
         <v>133.42499999999998</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E26" s="36">
         <f>104.9/(1-(L36/L35))</f>
         <v>131.125</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="36">
         <f>109.16/(1-(L36/L35))</f>
         <v>136.44999999999999</v>
       </c>
@@ -10384,10 +10468,10 @@
       <c r="I26" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="K26" s="39" t="s">
+      <c r="K26" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="L26" s="39" t="s">
+      <c r="L26" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -10398,7 +10482,7 @@
       <c r="B27" s="4">
         <v>0</v>
       </c>
-      <c r="C27" s="37">
+      <c r="C27" s="33">
         <f t="shared" si="0"/>
         <v>71.11666666666666</v>
       </c>
@@ -10420,7 +10504,7 @@
       <c r="I27" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="K27" s="38" t="s">
+      <c r="K27" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L27" s="4">
@@ -10434,7 +10518,7 @@
       <c r="B28" s="4">
         <v>0</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C28" s="33">
         <f t="shared" si="0"/>
         <v>79.123333333333335</v>
       </c>
@@ -10456,7 +10540,7 @@
       <c r="I28" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="K28" s="38" t="s">
+      <c r="K28" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L28" s="4">
@@ -10473,22 +10557,22 @@
       <c r="C29" s="18">
         <v>0</v>
       </c>
-      <c r="D29" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G29" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H29" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I29" s="35" t="s">
+      <c r="D29" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I29" s="31" t="s">
         <v>99</v>
       </c>
     </row>
@@ -10502,28 +10586,28 @@
       <c r="C30" s="18">
         <v>0</v>
       </c>
-      <c r="D30" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E30" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F30" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G30" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H30" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I30" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K30" s="39" t="s">
+      <c r="D30" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K30" s="35" t="s">
         <v>341</v>
       </c>
-      <c r="L30" s="39" t="s">
+      <c r="L30" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -10537,25 +10621,25 @@
       <c r="C31" s="18">
         <v>0</v>
       </c>
-      <c r="D31" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E31" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G31" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H31" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I31" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K31" s="38" t="s">
+      <c r="D31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K31" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L31" s="4">
@@ -10569,8 +10653,8 @@
       <c r="B32" s="4">
         <v>0</v>
       </c>
-      <c r="C32" s="37">
-        <f>AVERAGE(D32:F32)</f>
+      <c r="C32" s="33">
+        <f t="shared" ref="C32:C38" si="1">AVERAGE(D32:F32)</f>
         <v>198.85666666666668</v>
       </c>
       <c r="D32" s="4">
@@ -10591,7 +10675,7 @@
       <c r="I32" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="K32" s="38" t="s">
+      <c r="K32" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L32" s="4">
@@ -10599,14 +10683,14 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="37" t="s">
         <v>350</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
       </c>
-      <c r="C33" s="37">
-        <f>AVERAGE(D33:F33)</f>
+      <c r="C33" s="33">
+        <f t="shared" si="1"/>
         <v>384.70666666666671</v>
       </c>
       <c r="D33" s="4">
@@ -10638,8 +10722,8 @@
       <c r="B34" s="4">
         <v>0</v>
       </c>
-      <c r="C34" s="37">
-        <f>AVERAGE(D34:F34)</f>
+      <c r="C34" s="33">
+        <f t="shared" si="1"/>
         <v>221.41666666666666</v>
       </c>
       <c r="D34" s="4">
@@ -10660,10 +10744,10 @@
       <c r="I34" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="K34" s="39" t="s">
+      <c r="K34" s="35" t="s">
         <v>342</v>
       </c>
-      <c r="L34" s="39" t="s">
+      <c r="L34" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -10674,8 +10758,8 @@
       <c r="B35" s="4">
         <v>0</v>
       </c>
-      <c r="C35" s="37">
-        <f>AVERAGE(D35:F35)</f>
+      <c r="C35" s="33">
+        <f t="shared" si="1"/>
         <v>188.47</v>
       </c>
       <c r="D35" s="4">
@@ -10696,7 +10780,7 @@
       <c r="I35" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="K35" s="38" t="s">
+      <c r="K35" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L35" s="4">
@@ -10710,8 +10794,8 @@
       <c r="B36" s="4">
         <v>0</v>
       </c>
-      <c r="C36" s="37">
-        <f>AVERAGE(D36:F36)</f>
+      <c r="C36" s="33">
+        <f t="shared" si="1"/>
         <v>103.36</v>
       </c>
       <c r="D36" s="4">
@@ -10732,7 +10816,7 @@
       <c r="I36" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="K36" s="38" t="s">
+      <c r="K36" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L36" s="4">
@@ -10747,7 +10831,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="18">
-        <f>AVERAGE(D37:F37)</f>
+        <f t="shared" si="1"/>
         <v>90.63</v>
       </c>
       <c r="D37" s="4">
@@ -10776,8 +10860,8 @@
       <c r="B38" s="4">
         <v>0</v>
       </c>
-      <c r="C38" s="36">
-        <f>AVERAGE(D38:F38)</f>
+      <c r="C38" s="32">
+        <f t="shared" si="1"/>
         <v>33.056666666666665</v>
       </c>
       <c r="D38" s="4">
@@ -10798,10 +10882,10 @@
       <c r="I38" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="K38" s="39" t="s">
+      <c r="K38" s="35" t="s">
         <v>350</v>
       </c>
-      <c r="L38" s="39" t="s">
+      <c r="L38" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -10815,25 +10899,25 @@
       <c r="C39" s="18">
         <v>0</v>
       </c>
-      <c r="D39" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E39" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F39" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G39" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H39" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I39" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K39" s="38" t="s">
+      <c r="D39" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H39" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K39" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L39" s="4">
@@ -10847,7 +10931,7 @@
       <c r="B40" s="4">
         <v>0</v>
       </c>
-      <c r="C40" s="37">
+      <c r="C40" s="33">
         <f>AVERAGE(D40:F40)</f>
         <v>38.456666666666671</v>
       </c>
@@ -10869,7 +10953,7 @@
       <c r="I40" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="K40" s="38" t="s">
+      <c r="K40" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L40" s="4">
@@ -10886,22 +10970,22 @@
       <c r="C41" s="18">
         <v>0</v>
       </c>
-      <c r="D41" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E41" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F41" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G41" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H41" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I41" s="35" t="s">
+      <c r="D41" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I41" s="31" t="s">
         <v>99</v>
       </c>
     </row>
@@ -10915,39 +10999,39 @@
       <c r="C42" s="18">
         <v>0</v>
       </c>
-      <c r="D42" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E42" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F42" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G42" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H42" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I42" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K42" s="39" t="s">
+      <c r="D42" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G42" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I42" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K42" s="35" t="s">
         <v>364</v>
       </c>
-      <c r="L42" s="39" t="s">
+      <c r="L42" s="35" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="37" t="s">
         <v>364</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
       </c>
-      <c r="C43" s="37">
+      <c r="C43" s="33">
         <f>AVERAGE(D43:F43)</f>
         <v>852.2399999999999</v>
       </c>
@@ -10972,7 +11056,7 @@
       <c r="I43" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="K43" s="38" t="s">
+      <c r="K43" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L43" s="4">
@@ -10986,8 +11070,8 @@
       <c r="B44" s="4">
         <v>0</v>
       </c>
-      <c r="C44" s="37">
-        <f t="shared" ref="C44:C49" si="1">AVERAGE(D44:F44)</f>
+      <c r="C44" s="33">
+        <f t="shared" ref="C44:C49" si="2">AVERAGE(D44:F44)</f>
         <v>115.69999999999999</v>
       </c>
       <c r="D44" s="4">
@@ -11008,7 +11092,7 @@
       <c r="I44" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="K44" s="38" t="s">
+      <c r="K44" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L44" s="4">
@@ -11016,14 +11100,14 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="37" t="s">
         <v>366</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
       </c>
-      <c r="C45" s="37">
-        <f t="shared" si="1"/>
+      <c r="C45" s="33">
+        <f t="shared" si="2"/>
         <v>633.5866666666667</v>
       </c>
       <c r="D45" s="4">
@@ -11049,14 +11133,14 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="41" t="s">
+      <c r="A46" s="37" t="s">
         <v>367</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
       </c>
-      <c r="C46" s="37">
-        <f t="shared" si="1"/>
+      <c r="C46" s="33">
+        <f t="shared" si="2"/>
         <v>898.29333333333341</v>
       </c>
       <c r="D46" s="4">
@@ -11080,22 +11164,22 @@
       <c r="I46" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="K46" s="39" t="s">
+      <c r="K46" s="35" t="s">
         <v>366</v>
       </c>
-      <c r="L46" s="39" t="s">
+      <c r="L46" s="35" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="37" t="s">
         <v>368</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
       </c>
-      <c r="C47" s="37">
-        <f t="shared" si="1"/>
+      <c r="C47" s="33">
+        <f t="shared" si="2"/>
         <v>440.10666666666663</v>
       </c>
       <c r="D47" s="4">
@@ -11119,7 +11203,7 @@
       <c r="I47" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="K47" s="38" t="s">
+      <c r="K47" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L47" s="4">
@@ -11127,14 +11211,14 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="41" t="s">
+      <c r="A48" s="37" t="s">
         <v>369</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
       </c>
-      <c r="C48" s="37">
-        <f t="shared" si="1"/>
+      <c r="C48" s="33">
+        <f t="shared" si="2"/>
         <v>556.35333333333335</v>
       </c>
       <c r="D48" s="4">
@@ -11158,7 +11242,7 @@
       <c r="I48" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="K48" s="38" t="s">
+      <c r="K48" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L48" s="4">
@@ -11172,8 +11256,8 @@
       <c r="B49" s="4">
         <v>0</v>
       </c>
-      <c r="C49" s="37">
-        <f t="shared" si="1"/>
+      <c r="C49" s="33">
+        <f t="shared" si="2"/>
         <v>125.32333333333334</v>
       </c>
       <c r="D49" s="4">
@@ -11208,28 +11292,28 @@
       <c r="C50" s="18">
         <v>0</v>
       </c>
-      <c r="D50" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E50" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F50" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G50" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H50" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I50" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K50" s="39" t="s">
+      <c r="D50" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F50" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G50" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H50" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I50" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K50" s="35" t="s">
         <v>367</v>
       </c>
-      <c r="L50" s="39" t="s">
+      <c r="L50" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -11243,25 +11327,25 @@
       <c r="C51" s="18">
         <v>0</v>
       </c>
-      <c r="D51" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E51" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F51" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G51" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H51" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I51" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K51" s="38" t="s">
+      <c r="D51" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G51" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H51" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I51" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K51" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L51" s="4">
@@ -11278,25 +11362,25 @@
       <c r="C52" s="18">
         <v>0</v>
       </c>
-      <c r="D52" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E52" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F52" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G52" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H52" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I52" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K52" s="38" t="s">
+      <c r="D52" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F52" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G52" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H52" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I52" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K52" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L52" s="4">
@@ -11304,13 +11388,13 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="37" t="s">
         <v>374</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
       </c>
-      <c r="C53" s="37">
+      <c r="C53" s="33">
         <f>AVERAGE(D53:F53)</f>
         <v>496.45333333333332</v>
       </c>
@@ -11337,25 +11421,25 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="41" t="s">
+      <c r="A54" s="37" t="s">
         <v>375</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
       </c>
-      <c r="C54" s="37">
-        <f t="shared" ref="C54:C56" si="2">AVERAGE(D54:F54)</f>
+      <c r="C54" s="33">
+        <f t="shared" ref="C54:C56" si="3">AVERAGE(D54:F54)</f>
         <v>290.97777777777782</v>
       </c>
-      <c r="D54" s="40">
+      <c r="D54" s="36">
         <f>167.02/(1-(L68/L67))</f>
         <v>278.36666666666667</v>
       </c>
-      <c r="E54" s="40">
+      <c r="E54" s="36">
         <f>171.84/(1-(L68/L67))</f>
         <v>286.40000000000003</v>
       </c>
-      <c r="F54" s="40">
+      <c r="F54" s="36">
         <f>184.9/(1-(L68/L67))</f>
         <v>308.16666666666669</v>
       </c>
@@ -11368,10 +11452,10 @@
       <c r="I54" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="K54" s="39" t="s">
+      <c r="K54" s="35" t="s">
         <v>368</v>
       </c>
-      <c r="L54" s="39" t="s">
+      <c r="L54" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -11382,8 +11466,8 @@
       <c r="B55" s="4">
         <v>0</v>
       </c>
-      <c r="C55" s="37">
-        <f t="shared" si="2"/>
+      <c r="C55" s="33">
+        <f t="shared" si="3"/>
         <v>236.06333333333336</v>
       </c>
       <c r="D55" s="4">
@@ -11404,7 +11488,7 @@
       <c r="I55" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="K55" s="38" t="s">
+      <c r="K55" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L55" s="4">
@@ -11418,8 +11502,8 @@
       <c r="B56" s="4">
         <v>0</v>
       </c>
-      <c r="C56" s="37">
-        <f t="shared" si="2"/>
+      <c r="C56" s="33">
+        <f t="shared" si="3"/>
         <v>185.60333333333335</v>
       </c>
       <c r="D56" s="4">
@@ -11440,7 +11524,7 @@
       <c r="I56" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="K56" s="38" t="s">
+      <c r="K56" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L56" s="4">
@@ -11454,7 +11538,7 @@
       <c r="B57" s="4">
         <v>0</v>
       </c>
-      <c r="C57" s="37">
+      <c r="C57" s="33">
         <f>AVERAGE(D57:F57)</f>
         <v>125.89333333333333</v>
       </c>
@@ -11484,7 +11568,7 @@
       <c r="B58" s="4">
         <v>0</v>
       </c>
-      <c r="C58" s="37">
+      <c r="C58" s="33">
         <f>AVERAGE(D58:F58)</f>
         <v>91.566666666666663</v>
       </c>
@@ -11506,15 +11590,15 @@
       <c r="I58" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="K58" s="39" t="s">
+      <c r="K58" s="35" t="s">
         <v>369</v>
       </c>
-      <c r="L58" s="39" t="s">
+      <c r="L58" s="35" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="42" t="s">
+      <c r="A59" s="38" t="s">
         <v>392</v>
       </c>
       <c r="B59" s="4">
@@ -11523,25 +11607,25 @@
       <c r="C59" s="18">
         <v>0</v>
       </c>
-      <c r="D59" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E59" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F59" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G59" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H59" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I59" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K59" s="38" t="s">
+      <c r="D59" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E59" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G59" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H59" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I59" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K59" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L59" s="4">
@@ -11558,25 +11642,25 @@
       <c r="C60" s="18">
         <v>0</v>
       </c>
-      <c r="D60" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E60" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F60" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G60" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H60" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I60" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K60" s="38" t="s">
+      <c r="D60" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G60" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H60" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I60" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K60" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L60" s="4">
@@ -11593,22 +11677,22 @@
       <c r="C61" s="18">
         <v>0</v>
       </c>
-      <c r="D61" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="E61" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F61" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G61" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H61" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="I61" s="35" t="s">
+      <c r="D61" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E61" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G61" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H61" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="I61" s="31" t="s">
         <v>99</v>
       </c>
     </row>
@@ -11619,7 +11703,7 @@
       <c r="B62" s="4">
         <v>1</v>
       </c>
-      <c r="C62" s="37">
+      <c r="C62" s="33">
         <f>AVERAGE(D62:F62)</f>
         <v>300.90666666666669</v>
       </c>
@@ -11644,10 +11728,10 @@
       <c r="I62" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="K62" s="39" t="s">
+      <c r="K62" s="35" t="s">
         <v>374</v>
       </c>
-      <c r="L62" s="39" t="s">
+      <c r="L62" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -11658,8 +11742,8 @@
       <c r="B63" s="4">
         <v>0</v>
       </c>
-      <c r="C63" s="37">
-        <f t="shared" ref="C63:C67" si="3">AVERAGE(D63:F63)</f>
+      <c r="C63" s="33">
+        <f t="shared" ref="C63:C67" si="4">AVERAGE(D63:F63)</f>
         <v>222.65333333333334</v>
       </c>
       <c r="D63" s="4">
@@ -11680,7 +11764,7 @@
       <c r="I63" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="K63" s="38" t="s">
+      <c r="K63" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L63" s="4">
@@ -11694,8 +11778,8 @@
       <c r="B64" s="4">
         <v>0</v>
       </c>
-      <c r="C64" s="37">
-        <f t="shared" si="3"/>
+      <c r="C64" s="33">
+        <f t="shared" si="4"/>
         <v>200.62666666666667</v>
       </c>
       <c r="D64" s="4">
@@ -11716,7 +11800,7 @@
       <c r="I64" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="K64" s="38" t="s">
+      <c r="K64" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L64" s="4">
@@ -11730,26 +11814,26 @@
       <c r="B65" s="4">
         <v>0</v>
       </c>
-      <c r="C65" s="37">
-        <f t="shared" si="3"/>
+      <c r="C65" s="33">
+        <f t="shared" si="4"/>
         <v>138.66</v>
       </c>
-      <c r="D65" s="35">
+      <c r="D65" s="31">
         <v>133.03</v>
       </c>
-      <c r="E65" s="35">
+      <c r="E65" s="31">
         <v>149.44</v>
       </c>
-      <c r="F65" s="35">
+      <c r="F65" s="31">
         <v>133.51</v>
       </c>
-      <c r="G65" s="35" t="s">
+      <c r="G65" s="31" t="s">
         <v>390</v>
       </c>
-      <c r="H65" s="35" t="s">
+      <c r="H65" s="31" t="s">
         <v>391</v>
       </c>
-      <c r="I65" s="35" t="s">
+      <c r="I65" s="31" t="s">
         <v>392</v>
       </c>
     </row>
@@ -11760,8 +11844,8 @@
       <c r="B66" s="4">
         <v>0</v>
       </c>
-      <c r="C66" s="37">
-        <f t="shared" si="3"/>
+      <c r="C66" s="33">
+        <f t="shared" si="4"/>
         <v>85.34999999999998</v>
       </c>
       <c r="D66" s="4">
@@ -11782,10 +11866,10 @@
       <c r="I66" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="K66" s="39" t="s">
+      <c r="K66" s="35" t="s">
         <v>375</v>
       </c>
-      <c r="L66" s="39" t="s">
+      <c r="L66" s="35" t="s">
         <v>446</v>
       </c>
     </row>
@@ -11796,8 +11880,8 @@
       <c r="B67" s="4">
         <v>0</v>
       </c>
-      <c r="C67" s="37">
-        <f t="shared" si="3"/>
+      <c r="C67" s="33">
+        <f t="shared" si="4"/>
         <v>60.026666666666664</v>
       </c>
       <c r="D67" s="4">
@@ -11818,7 +11902,7 @@
       <c r="I67" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="K67" s="38" t="s">
+      <c r="K67" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L67" s="4">
@@ -11826,7 +11910,7 @@
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K68" s="38" t="s">
+      <c r="K68" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L68" s="4">
@@ -11834,15 +11918,15 @@
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K70" s="39" t="s">
+      <c r="K70" s="35" t="s">
         <v>391</v>
       </c>
-      <c r="L70" s="39" t="s">
+      <c r="L70" s="35" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K71" s="38" t="s">
+      <c r="K71" s="34" t="s">
         <v>445</v>
       </c>
       <c r="L71" s="4">
@@ -11850,7 +11934,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K72" s="38" t="s">
+      <c r="K72" s="34" t="s">
         <v>447</v>
       </c>
       <c r="L72" s="4">

</xml_diff>

<commit_message>
updating sample IDs for carbon
</commit_message>
<xml_diff>
--- a/GSD/Water Samples/LaJara_LISST_GSD_Summer2023.xlsx
+++ b/GSD/Water Samples/LaJara_LISST_GSD_Summer2023.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Water Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587FDC4B-1C7C-4689-AC67-4F0C3BDC499A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1964EDAB-D60A-481C-BFE0-F8216B20E2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5952B5DA-6B13-43D1-9193-1BE03F62DE4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5952B5DA-6B13-43D1-9193-1BE03F62DE4B}"/>
   </bookViews>
   <sheets>
     <sheet name="&quot;Storm&quot; 1" sheetId="2" r:id="rId1"/>
     <sheet name="&quot;Storm&quot; 2" sheetId="6" r:id="rId2"/>
     <sheet name="&quot;Storm&quot; 3" sheetId="7" r:id="rId3"/>
-    <sheet name="Grab Samples" sheetId="5" r:id="rId4"/>
-    <sheet name="&quot;Storm&quot; 4" sheetId="8" r:id="rId5"/>
+    <sheet name="&quot;Storm&quot; 4" sheetId="8" r:id="rId4"/>
+    <sheet name="Grab Samples" sheetId="5" r:id="rId5"/>
     <sheet name="Flood Experiments" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="499">
   <si>
     <t>Dilutions</t>
   </si>
@@ -1531,6 +1531,12 @@
   </si>
   <si>
     <t xml:space="preserve">Dil Conc </t>
+  </si>
+  <si>
+    <t>LAB ID</t>
+  </si>
+  <si>
+    <t>DOWN 7</t>
   </si>
 </sst>
 </file>
@@ -1588,7 +1594,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1916,11 +1922,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2044,9 +2061,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2085,12 +2099,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2109,13 +2117,43 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2432,10 +2470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CFA7B-6AB5-4D15-9587-78BC8AED2040}">
-  <dimension ref="A1:P135"/>
+  <dimension ref="A1:Q135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N120" sqref="N120"/>
+    <sheetView topLeftCell="C99" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P122" sqref="P122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2455,12 +2493,12 @@
     <col min="16" max="16" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2476,15 +2514,18 @@
       <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="N2" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="60" t="s">
+      <c r="O2" s="67"/>
+      <c r="P2" s="57" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q2" s="31" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>44</v>
       </c>
@@ -2515,21 +2556,24 @@
       <c r="J3" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="K3" s="50" t="s">
+      <c r="K3" s="49" t="s">
         <v>492</v>
       </c>
-      <c r="N3" s="55" t="s">
+      <c r="N3" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="O3" s="56">
+      <c r="O3" s="55">
         <v>45136.636111111111</v>
       </c>
-      <c r="P3" s="57">
+      <c r="P3" s="56">
         <f>AVERAGE(H4:H6)</f>
         <v>327.45333333333332</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="18">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -2551,7 +2595,7 @@
       <c r="G4" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="46">
+      <c r="H4" s="45">
         <f>K4/(1-($J$4/$I$4))</f>
         <v>320.83999999999997</v>
       </c>
@@ -2567,15 +2611,18 @@
       <c r="N4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="O4" s="53">
+      <c r="O4" s="52">
         <v>45136.646527777775</v>
       </c>
-      <c r="P4" s="54">
+      <c r="P4" s="53">
         <f>AVERAGE(H10:H12)</f>
         <v>241.80933333333334</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="18">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
@@ -2609,15 +2656,18 @@
       <c r="N5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="53">
+      <c r="O5" s="52">
         <v>45136.656944444447</v>
       </c>
-      <c r="P5" s="54">
+      <c r="P5" s="53">
         <f>AVERAGE(E9:E12)</f>
         <v>158.52499999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q5" s="18">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>74</v>
       </c>
@@ -2639,27 +2689,30 @@
       <c r="G6" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="H6" s="48">
+      <c r="H6" s="47">
         <f>K6/(1-($J$4/$I$4))</f>
         <v>333.42666666666668</v>
       </c>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="51">
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="50">
         <v>250.07</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="O6" s="53">
+      <c r="O6" s="52">
         <v>45136.667361111111</v>
       </c>
-      <c r="P6" s="54">
+      <c r="P6" s="53">
         <f>AVERAGE(E13:E17)</f>
         <v>132.47200000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6" s="18">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>74</v>
       </c>
@@ -2684,15 +2737,18 @@
       <c r="N7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="O7" s="53">
+      <c r="O7" s="52">
         <v>45136.677777777775</v>
       </c>
-      <c r="P7" s="54">
+      <c r="P7" s="53">
         <f>AVERAGE(E18:E20)</f>
         <v>98.909999999999982</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q7" s="18">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>74</v>
       </c>
@@ -2717,15 +2773,18 @@
       <c r="N8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="O8" s="53">
+      <c r="O8" s="52">
         <v>45136.688194444447</v>
       </c>
-      <c r="P8" s="54">
+      <c r="P8" s="53">
         <f>AVERAGE(E21:E23)</f>
         <v>90.356666666666669</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="18">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>50</v>
       </c>
@@ -2747,7 +2806,7 @@
       <c r="G9" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="45" t="s">
         <v>74</v>
       </c>
       <c r="I9" s="16" t="s">
@@ -2756,21 +2815,24 @@
       <c r="J9" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="K9" s="47" t="s">
+      <c r="K9" s="46" t="s">
         <v>492</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="53">
+      <c r="O9" s="52">
         <v>45136.698611111111</v>
       </c>
       <c r="P9" s="4">
         <f>AVERAGE(E24:E28)</f>
         <v>84.561999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="18">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>50</v>
       </c>
@@ -2808,15 +2870,18 @@
       <c r="N10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="O10" s="53">
+      <c r="O10" s="52">
         <v>45136.709027777775</v>
       </c>
       <c r="P10" s="4">
         <f>AVERAGE(E29:E34)</f>
         <v>69.045000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
@@ -2842,23 +2907,26 @@
         <f t="shared" ref="H11:H12" si="0">K11/(1-($J$10/$I$10))</f>
         <v>232.309</v>
       </c>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
       <c r="K11" s="5">
         <v>211.19</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="O11" s="53">
+      <c r="O11" s="52">
         <v>45136.719444444447</v>
       </c>
       <c r="P11" s="4">
         <f>AVERAGE(E35:E39)</f>
         <v>59.009999999999991</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q11" s="18">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>50</v>
       </c>
@@ -2880,27 +2948,30 @@
       <c r="G12" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="47">
         <f t="shared" si="0"/>
         <v>250.602</v>
       </c>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="51">
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="50">
         <v>227.82</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="O12" s="53">
+      <c r="O12" s="52">
         <v>45136.729861111111</v>
       </c>
       <c r="P12" s="4">
         <f>AVERAGE(E40:E44)</f>
         <v>50.82</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>55</v>
       </c>
@@ -2925,15 +2996,18 @@
       <c r="N13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="O13" s="53">
+      <c r="O13" s="52">
         <v>45136.740277777775</v>
       </c>
       <c r="P13" s="4">
         <f>AVERAGE(E45:E49)</f>
         <v>42.72</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="18">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>55</v>
       </c>
@@ -2958,15 +3032,18 @@
       <c r="N14" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="O14" s="53">
+      <c r="O14" s="52">
         <v>45136.750694444447</v>
       </c>
       <c r="P14" s="4">
         <f>AVERAGE(E50:E53)</f>
         <v>48.344999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>55</v>
       </c>
@@ -2991,15 +3068,18 @@
       <c r="N15" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="O15" s="53">
+      <c r="O15" s="52">
         <v>45136.761111111111</v>
       </c>
       <c r="P15" s="4">
         <f>AVERAGE(E54:E58)</f>
         <v>74.881999999999991</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>55</v>
       </c>
@@ -3024,15 +3104,18 @@
       <c r="N16" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="O16" s="53">
+      <c r="O16" s="52">
         <v>45136.771527777775</v>
       </c>
       <c r="P16" s="4">
         <f>AVERAGE(E59:E63)</f>
         <v>98.145999999999987</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="18">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>55</v>
       </c>
@@ -3057,15 +3140,18 @@
       <c r="N17" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="O17" s="53">
+      <c r="O17" s="52">
         <v>45136.781944444447</v>
       </c>
       <c r="P17" s="4">
         <f>AVERAGE(E64:E68)</f>
         <v>91.213999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>59</v>
       </c>
@@ -3090,15 +3176,18 @@
       <c r="N18" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="O18" s="53">
+      <c r="O18" s="52">
         <v>45136.792361111111</v>
       </c>
       <c r="P18" s="4">
         <f>AVERAGE(E69:E73)</f>
         <v>74.50800000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>59</v>
       </c>
@@ -3123,15 +3212,18 @@
       <c r="N19" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="O19" s="53">
+      <c r="O19" s="52">
         <v>45136.802777777775</v>
       </c>
       <c r="P19" s="4">
         <f>AVERAGE(E74:E78)</f>
         <v>81.948000000000008</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>59</v>
       </c>
@@ -3157,15 +3249,18 @@
       <c r="N20" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="O20" s="53">
+      <c r="O20" s="52">
         <v>45136.813194444447</v>
       </c>
       <c r="P20" s="4">
         <f>AVERAGE(E79:E83)</f>
         <v>52.010000000000005</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>61</v>
       </c>
@@ -3190,15 +3285,18 @@
       <c r="N21" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="O21" s="53">
+      <c r="O21" s="52">
         <v>45136.823611111111</v>
       </c>
-      <c r="P21" s="54">
+      <c r="P21" s="53">
         <f>AVERAGE(E84:E89)</f>
         <v>52.246666666666663</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>61</v>
       </c>
@@ -3223,15 +3321,18 @@
       <c r="N22" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="O22" s="53">
+      <c r="O22" s="52">
         <v>45136.834027777775</v>
       </c>
       <c r="P22" s="4">
         <f>AVERAGE(E90:E95)</f>
         <v>48.755000000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>61</v>
       </c>
@@ -3256,15 +3357,18 @@
       <c r="N23" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="O23" s="53">
+      <c r="O23" s="52">
         <v>45136.844444444447</v>
       </c>
       <c r="P23" s="4">
         <f>AVERAGE(E96:E100)</f>
         <v>48.024000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>63</v>
       </c>
@@ -3289,15 +3393,18 @@
       <c r="N24" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="O24" s="53">
+      <c r="O24" s="52">
         <v>45136.854861111111</v>
       </c>
       <c r="P24" s="4">
         <f>AVERAGE(E101:E105)</f>
         <v>44.088000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>63</v>
       </c>
@@ -3322,14 +3429,17 @@
       <c r="N25" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="O25" s="53">
+      <c r="O25" s="52">
         <v>45136.865277777775</v>
       </c>
       <c r="P25" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>63</v>
       </c>
@@ -3354,15 +3464,18 @@
       <c r="N26" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="O26" s="53">
+      <c r="O26" s="52">
         <v>45136.875694444447</v>
       </c>
-      <c r="P26" s="54">
+      <c r="P26" s="53">
         <f>AVERAGE(E110,E107:E108)</f>
         <v>37.736666666666665</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>63</v>
       </c>
@@ -3385,7 +3498,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>63</v>
       </c>
@@ -3408,7 +3521,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>65</v>
       </c>
@@ -3431,7 +3544,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>65</v>
       </c>
@@ -3454,7 +3567,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>65</v>
       </c>
@@ -3477,7 +3590,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>65</v>
       </c>
@@ -4972,7 +5085,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>110</v>
       </c>
@@ -4995,7 +5108,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>110</v>
       </c>
@@ -5018,7 +5131,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>110</v>
       </c>
@@ -5041,7 +5154,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>110</v>
       </c>
@@ -5064,7 +5177,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>111</v>
       </c>
@@ -5087,7 +5200,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>111</v>
       </c>
@@ -5110,7 +5223,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>111</v>
       </c>
@@ -5133,7 +5246,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>111</v>
       </c>
@@ -5156,7 +5269,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>111</v>
       </c>
@@ -5178,15 +5291,18 @@
       <c r="G105" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="N105" s="66" t="s">
+      <c r="N105" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="O105" s="67"/>
-      <c r="P105" s="68" t="s">
+      <c r="O105" s="69"/>
+      <c r="P105" s="63" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q105" s="31" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>112</v>
       </c>
@@ -5214,12 +5330,15 @@
       <c r="O106" s="14">
         <v>45136.629861111112</v>
       </c>
-      <c r="P106" s="54">
+      <c r="P106" s="53">
         <f>AVERAGE(H113:H116)</f>
         <v>223.61406716417912</v>
       </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q106" s="4">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>113</v>
       </c>
@@ -5247,12 +5366,15 @@
       <c r="O107" s="14">
         <v>45136.640277777777</v>
       </c>
-      <c r="P107" s="54">
+      <c r="P107" s="53">
         <f>AVERAGE(H118:H122,E117)</f>
         <v>200.69044776119404</v>
       </c>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q107" s="4">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>113</v>
       </c>
@@ -5280,12 +5402,15 @@
       <c r="O108" s="14">
         <v>45136.650694444441</v>
       </c>
-      <c r="P108" s="54">
+      <c r="P108" s="53">
         <f>AVERAGE(E123,E124,E125,H127)</f>
         <v>231.91373134328356</v>
       </c>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q108" s="4">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>113</v>
       </c>
@@ -5317,8 +5442,11 @@
         <f>AVERAGE(E127:E130)</f>
         <v>233.2525</v>
       </c>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q109" s="4">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>113</v>
       </c>
@@ -5350,8 +5478,11 @@
         <f>AVERAGE(E131:E135)</f>
         <v>124.55999999999999</v>
       </c>
-    </row>
-    <row r="111" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q110" s="4">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>113</v>
       </c>
@@ -5374,7 +5505,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>17</v>
       </c>
@@ -5396,7 +5527,7 @@
       <c r="G112" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="H112" s="63" t="s">
+      <c r="H112" s="60" t="s">
         <v>232</v>
       </c>
       <c r="I112" s="1" t="s">
@@ -5405,7 +5536,7 @@
       <c r="J112" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="K112" s="47" t="s">
+      <c r="K112" s="46" t="s">
         <v>492</v>
       </c>
       <c r="L112" s="22" t="s">
@@ -5434,7 +5565,7 @@
       <c r="G113" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="H113" s="64">
+      <c r="H113" s="61">
         <f>K113/(1-($J$113/$I$113))</f>
         <v>220.37910447761195</v>
       </c>
@@ -5470,12 +5601,12 @@
       <c r="G114" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="H114" s="64">
+      <c r="H114" s="61">
         <f t="shared" ref="H114:H115" si="1">K114/(1-($J$113/$I$113))</f>
         <v>224.91940298507467</v>
       </c>
-      <c r="I114" s="45"/>
-      <c r="J114" s="45"/>
+      <c r="I114" s="44"/>
+      <c r="J114" s="44"/>
       <c r="K114" s="5">
         <v>128.80000000000001</v>
       </c>
@@ -5502,12 +5633,12 @@
       <c r="G115" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="H115" s="64">
+      <c r="H115" s="61">
         <f t="shared" si="1"/>
         <v>222.82388059701492</v>
       </c>
-      <c r="I115" s="45"/>
-      <c r="J115" s="45"/>
+      <c r="I115" s="44"/>
+      <c r="J115" s="44"/>
       <c r="K115" s="5">
         <v>127.6</v>
       </c>
@@ -5534,13 +5665,13 @@
       <c r="G116" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="H116" s="65">
+      <c r="H116" s="62">
         <f>K116/(1-($J$113/$I$113))</f>
         <v>226.33388059701497</v>
       </c>
-      <c r="I116" s="52"/>
-      <c r="J116" s="52"/>
-      <c r="K116" s="51">
+      <c r="I116" s="51"/>
+      <c r="J116" s="51"/>
+      <c r="K116" s="50">
         <v>129.61000000000001</v>
       </c>
     </row>
@@ -5566,7 +5697,7 @@
       <c r="G117" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="H117" s="63" t="s">
+      <c r="H117" s="60" t="s">
         <v>200</v>
       </c>
       <c r="I117" s="1" t="s">
@@ -5575,7 +5706,7 @@
       <c r="J117" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="K117" s="47" t="s">
+      <c r="K117" s="46" t="s">
         <v>496</v>
       </c>
       <c r="L117" s="22" t="s">
@@ -5604,7 +5735,7 @@
       <c r="G118" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="H118" s="64">
+      <c r="H118" s="61">
         <f>K118/(1-($J$118/$I$118))</f>
         <v>155.10358208955225</v>
       </c>
@@ -5640,12 +5771,12 @@
       <c r="G119" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="H119" s="64">
+      <c r="H119" s="61">
         <f t="shared" ref="H119:H122" si="2">K119/(1-($J$118/$I$118))</f>
         <v>183.72492537313434</v>
       </c>
-      <c r="I119" s="45"/>
-      <c r="J119" s="45"/>
+      <c r="I119" s="44"/>
+      <c r="J119" s="44"/>
       <c r="K119" s="5">
         <v>105.21</v>
       </c>
@@ -5672,12 +5803,12 @@
       <c r="G120" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="H120" s="64">
+      <c r="H120" s="61">
         <f t="shared" si="2"/>
         <v>215.71656716417911</v>
       </c>
-      <c r="I120" s="45"/>
-      <c r="J120" s="45"/>
+      <c r="I120" s="44"/>
+      <c r="J120" s="44"/>
       <c r="K120" s="5">
         <v>123.53</v>
       </c>
@@ -5704,12 +5835,12 @@
       <c r="G121" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="H121" s="64">
+      <c r="H121" s="61">
         <f t="shared" si="2"/>
         <v>204.62776119402989</v>
       </c>
-      <c r="I121" s="45"/>
-      <c r="J121" s="45"/>
+      <c r="I121" s="44"/>
+      <c r="J121" s="44"/>
       <c r="K121" s="5">
         <v>117.18</v>
       </c>
@@ -5736,13 +5867,13 @@
       <c r="G122" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="H122" s="65">
+      <c r="H122" s="62">
         <f t="shared" si="2"/>
         <v>195.45985074626867</v>
       </c>
-      <c r="I122" s="52"/>
-      <c r="J122" s="52"/>
-      <c r="K122" s="51">
+      <c r="I122" s="51"/>
+      <c r="J122" s="51"/>
+      <c r="K122" s="50">
         <v>111.93</v>
       </c>
     </row>
@@ -5837,7 +5968,7 @@
       <c r="G126" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="H126" s="61" t="s">
+      <c r="H126" s="58" t="s">
         <v>244</v>
       </c>
       <c r="I126" s="4" t="s">
@@ -5872,7 +6003,7 @@
       <c r="G127" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="H127" s="62">
+      <c r="H127" s="59">
         <f>K127/(1-($J$127/$I$127))</f>
         <v>193.08492537313433</v>
       </c>
@@ -6082,10 +6213,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEA57E8-AC6C-4413-9DB1-76B8A0DB268F}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6097,14 +6228,17 @@
     <col min="5" max="5" width="20.140625" style="12" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" style="12"/>
     <col min="7" max="7" width="13.42578125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -6120,8 +6254,18 @@
       <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="65"/>
+      <c r="K2" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>17</v>
       </c>
@@ -6143,8 +6287,21 @@
       <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="71">
+        <v>45151.78125</v>
+      </c>
+      <c r="K3" s="1">
+        <f>AVERAGE(E3:E6)</f>
+        <v>210.45750000000001</v>
+      </c>
+      <c r="L3" s="4">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -6166,8 +6323,21 @@
       <c r="G4" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="9">
+        <v>45151.790277777778</v>
+      </c>
+      <c r="K4" s="4">
+        <f>AVERAGE(E7:E11)</f>
+        <v>116.06599999999999</v>
+      </c>
+      <c r="L4" s="4">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -6189,8 +6359,21 @@
       <c r="G5" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="9">
+        <v>45151.793055555558</v>
+      </c>
+      <c r="K5" s="4">
+        <f>AVERAGE(E12:E15)</f>
+        <v>113.25749999999999</v>
+      </c>
+      <c r="L5" s="4">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -6212,8 +6395,21 @@
       <c r="G6" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="9">
+        <v>45151.798611111109</v>
+      </c>
+      <c r="K6" s="4">
+        <f>AVERAGE(E17:E20)</f>
+        <v>81.149999999999991</v>
+      </c>
+      <c r="L6" s="4">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -6235,8 +6431,21 @@
       <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="70">
+        <v>45151.876388888886</v>
+      </c>
+      <c r="K7" s="48">
+        <f>AVERAGE(E21:E24)</f>
+        <v>56.15</v>
+      </c>
+      <c r="L7" s="4">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -6259,7 +6468,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
@@ -6281,8 +6490,18 @@
       <c r="G9" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="72"/>
+      <c r="K9" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -6304,8 +6523,21 @@
       <c r="G10" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="73">
+        <v>45151.78125</v>
+      </c>
+      <c r="K10" s="1">
+        <f>AVERAGE(E26:E30)</f>
+        <v>183.80800000000002</v>
+      </c>
+      <c r="L10" s="4">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -6327,8 +6559,21 @@
       <c r="G11" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="9">
+        <v>45151.791666666664</v>
+      </c>
+      <c r="K11" s="4">
+        <f>AVERAGE(E31:E35)</f>
+        <v>83.527999999999992</v>
+      </c>
+      <c r="L11" s="4">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -6350,8 +6595,21 @@
       <c r="G12" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="9">
+        <v>45151.802083333336</v>
+      </c>
+      <c r="K12" s="4">
+        <f>AVERAGE(E36:E39)</f>
+        <v>72.105000000000004</v>
+      </c>
+      <c r="L12" s="4">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -6373,8 +6631,21 @@
       <c r="G13" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="9">
+        <v>45151.8125</v>
+      </c>
+      <c r="K13" s="30">
+        <f>AVERAGE(E40:E42)</f>
+        <v>67.606666666666669</v>
+      </c>
+      <c r="L13" s="4">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -6396,8 +6667,21 @@
       <c r="G14" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="9">
+        <v>45151.822916666664</v>
+      </c>
+      <c r="K14" s="4">
+        <f>AVERAGE(E44)</f>
+        <v>70.3</v>
+      </c>
+      <c r="L14" s="4">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -6419,8 +6703,21 @@
       <c r="G15" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="9">
+        <v>45151.833333333336</v>
+      </c>
+      <c r="K15" s="4">
+        <f>AVERAGE(E45)</f>
+        <v>67.88</v>
+      </c>
+      <c r="L15" s="4">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -6442,8 +6739,21 @@
       <c r="G16" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="9">
+        <v>45151.84375</v>
+      </c>
+      <c r="K16" s="4">
+        <f>AVERAGE(E46)</f>
+        <v>84.66</v>
+      </c>
+      <c r="L16" s="4">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -6465,8 +6775,21 @@
       <c r="G17" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" s="9">
+        <v>45151.854166666664</v>
+      </c>
+      <c r="K17" s="4">
+        <f>AVERAGE(E47)</f>
+        <v>67.569999999999993</v>
+      </c>
+      <c r="L17" s="4">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -6488,8 +6811,21 @@
       <c r="G18" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="9">
+        <v>45151.864583333336</v>
+      </c>
+      <c r="K18" s="4">
+        <f>AVERAGE(E48:E52)</f>
+        <v>54.936</v>
+      </c>
+      <c r="L18" s="4">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
@@ -6511,8 +6847,21 @@
       <c r="G19" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" s="9">
+        <v>45151.875</v>
+      </c>
+      <c r="K19" s="4">
+        <f>AVERAGE(E53:E57)</f>
+        <v>75.337999999999994</v>
+      </c>
+      <c r="L19" s="4">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -6534,8 +6883,21 @@
       <c r="G20" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="9">
+        <v>45151.885416666664</v>
+      </c>
+      <c r="K20" s="4">
+        <f>AVERAGE(E58:E62)</f>
+        <v>59.165999999999997</v>
+      </c>
+      <c r="L20" s="4">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -6557,8 +6919,21 @@
       <c r="G21" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="J21" s="70">
+        <v>45151.895833333336</v>
+      </c>
+      <c r="K21" s="48">
+        <f>AVERAGE(E63:E67)</f>
+        <v>50.773999999999994</v>
+      </c>
+      <c r="L21" s="4">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -6581,7 +6956,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -6604,7 +6979,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -6627,7 +7002,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
@@ -6650,7 +7025,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>44</v>
       </c>
@@ -6673,7 +7048,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>44</v>
       </c>
@@ -6696,7 +7071,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>44</v>
       </c>
@@ -6719,7 +7094,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>44</v>
       </c>
@@ -6742,7 +7117,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>74</v>
       </c>
@@ -6765,7 +7140,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>74</v>
       </c>
@@ -7590,8 +7965,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7599,10 +7976,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA95C67-CE3C-4E97-BF30-FAEAA97B4B4A}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7614,14 +7991,18 @@
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="64" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -7637,8 +8018,18 @@
       <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="J2" s="65"/>
+      <c r="K2" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>44</v>
       </c>
@@ -7658,8 +8049,19 @@
       <c r="G3" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="4">
+        <f>AVERAGE(E3:E7)</f>
+        <v>232.05200000000005</v>
+      </c>
+      <c r="L3" s="4">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -7679,8 +8081,19 @@
       <c r="G4" s="5" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="4">
+        <f>AVERAGE(E8:E12)</f>
+        <v>143.89599999999999</v>
+      </c>
+      <c r="L4" s="4">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
@@ -7700,8 +8113,19 @@
       <c r="G5" s="5" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="4">
+        <f>AVERAGE(E13:E17)</f>
+        <v>104.006</v>
+      </c>
+      <c r="L5" s="4">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
@@ -7721,8 +8145,19 @@
       <c r="G6" s="5" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="4">
+        <f>AVERAGE(E18:E22)</f>
+        <v>88.143999999999977</v>
+      </c>
+      <c r="L6" s="4">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>44</v>
       </c>
@@ -7742,8 +8177,19 @@
       <c r="G7" s="5" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="4">
+        <f>AVERAGE(E23:E27)</f>
+        <v>92.256</v>
+      </c>
+      <c r="L7" s="4">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>74</v>
       </c>
@@ -7763,8 +8209,19 @@
       <c r="G8" s="5" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="4">
+        <f>AVERAGE(E28:E32)</f>
+        <v>87.688000000000002</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>74</v>
       </c>
@@ -7784,8 +8241,19 @@
       <c r="G9" s="5" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="4">
+        <f>AVERAGE(E33:E37)</f>
+        <v>95.621999999999986</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>74</v>
       </c>
@@ -7805,8 +8273,19 @@
       <c r="G10" s="5" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="4">
+        <f>AVERAGE(E38:E42)</f>
+        <v>82.494</v>
+      </c>
+      <c r="L10" s="4">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>74</v>
       </c>
@@ -7826,8 +8305,19 @@
       <c r="G11" s="5" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="4">
+        <f>AVERAGE(E43:E48)</f>
+        <v>77.09</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>74</v>
       </c>
@@ -7847,8 +8337,19 @@
       <c r="G12" s="5" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="4">
+        <f>AVERAGE(E49:E52)</f>
+        <v>69.39500000000001</v>
+      </c>
+      <c r="L12" s="4">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>50</v>
       </c>
@@ -7868,8 +8369,19 @@
       <c r="G13" s="5" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="4">
+        <f>AVERAGE(E53:E57)</f>
+        <v>65.813999999999993</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>50</v>
       </c>
@@ -7889,8 +8401,19 @@
       <c r="G14" s="5" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="4">
+        <f>AVERAGE(E58:E59)</f>
+        <v>79.97</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>50</v>
       </c>
@@ -7910,8 +8433,18 @@
       <c r="G15" s="5" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>50</v>
       </c>
@@ -8836,254 +9369,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20B0DB3-58B5-463D-B8A3-53DC39E150A4}">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="15">
-        <v>45120</v>
-      </c>
-      <c r="C3" s="16">
-        <v>0</v>
-      </c>
-      <c r="D3" s="16">
-        <v>96.1</v>
-      </c>
-      <c r="E3" s="16">
-        <v>79</v>
-      </c>
-      <c r="F3" s="16">
-        <v>294.74</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6">
-        <v>45120</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>96</v>
-      </c>
-      <c r="E4" s="4">
-        <v>67.209999999999994</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="6">
-        <v>45120</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>96.6</v>
-      </c>
-      <c r="E5" s="4">
-        <v>61.49</v>
-      </c>
-      <c r="F5" s="4">
-        <v>166.87</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="6">
-        <v>45120</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>96.9</v>
-      </c>
-      <c r="E6" s="4">
-        <v>56.77</v>
-      </c>
-      <c r="F6" s="4">
-        <v>93.57</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6">
-        <v>45127</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>98</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="6">
-        <v>45127</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>98</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="6">
-        <v>45146</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>98</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45146</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
-        <v>98</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD81FE8B-68DD-410E-8571-EE78EDCA3E1E}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9128,6 +9427,9 @@
       <c r="I1" s="35" t="s">
         <v>433</v>
       </c>
+      <c r="J1" s="74" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="2" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -9158,6 +9460,7 @@
       <c r="I2" s="25" t="s">
         <v>451</v>
       </c>
+      <c r="J2" s="44"/>
     </row>
     <row r="3" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -9188,6 +9491,7 @@
       <c r="I3" s="25" t="s">
         <v>454</v>
       </c>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
@@ -9218,6 +9522,7 @@
       <c r="I4" s="4" t="s">
         <v>469</v>
       </c>
+      <c r="J4" s="44"/>
     </row>
     <row r="5" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
@@ -9248,6 +9553,7 @@
       <c r="I5" s="25" t="s">
         <v>471</v>
       </c>
+      <c r="J5" s="44"/>
     </row>
     <row r="6" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
@@ -9278,6 +9584,7 @@
       <c r="I6" s="4" t="s">
         <v>473</v>
       </c>
+      <c r="J6" s="44"/>
     </row>
     <row r="7" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
@@ -9308,6 +9615,7 @@
       <c r="I7" s="4" t="s">
         <v>475</v>
       </c>
+      <c r="J7" s="44"/>
     </row>
     <row r="8" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
@@ -9338,6 +9646,7 @@
       <c r="I8" s="4" t="s">
         <v>477</v>
       </c>
+      <c r="J8" s="44"/>
     </row>
     <row r="9" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
@@ -9368,6 +9677,7 @@
       <c r="I9" s="4" t="s">
         <v>479</v>
       </c>
+      <c r="J9" s="44"/>
     </row>
     <row r="10" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
@@ -9398,6 +9708,7 @@
       <c r="I10" s="25" t="s">
         <v>99</v>
       </c>
+      <c r="J10" s="44"/>
     </row>
     <row r="11" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
@@ -9440,6 +9751,9 @@
       <c r="I12" s="25" t="s">
         <v>481</v>
       </c>
+      <c r="J12" s="4">
+        <v>484</v>
+      </c>
     </row>
     <row r="13" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
@@ -9470,6 +9784,9 @@
       <c r="I13" s="25" t="s">
         <v>483</v>
       </c>
+      <c r="J13" s="4">
+        <v>485</v>
+      </c>
     </row>
     <row r="14" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
@@ -9500,6 +9817,9 @@
       <c r="I14" s="25" t="s">
         <v>485</v>
       </c>
+      <c r="J14" s="4">
+        <v>486</v>
+      </c>
     </row>
     <row r="15" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
@@ -9530,6 +9850,9 @@
       <c r="I15" s="4" t="s">
         <v>487</v>
       </c>
+      <c r="J15" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="16" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
@@ -9560,8 +9883,11 @@
       <c r="I16" s="4" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="4">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -9590,19 +9916,27 @@
       <c r="I17" s="25" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="4">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>498</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
@@ -9613,7 +9947,7 @@
       <c r="H19" s="38"/>
       <c r="I19" s="38"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
@@ -9624,7 +9958,7 @@
       <c r="H20" s="38"/>
       <c r="I20" s="38"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="33"/>
       <c r="B21" s="33"/>
       <c r="C21" s="33"/>
@@ -9635,7 +9969,7 @@
       <c r="H21" s="38"/>
       <c r="I21" s="38"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
@@ -9646,7 +9980,7 @@
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="33"/>
       <c r="C23" s="41"/>
@@ -9657,7 +9991,7 @@
       <c r="H23" s="33"/>
       <c r="I23" s="33"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
       <c r="B24" s="33"/>
       <c r="C24" s="41"/>
@@ -9668,7 +10002,7 @@
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="33"/>
       <c r="C25" s="41"/>
@@ -9679,7 +10013,7 @@
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="33"/>
       <c r="C26" s="41"/>
@@ -9690,7 +10024,7 @@
       <c r="H26" s="33"/>
       <c r="I26" s="33"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
       <c r="B27" s="33"/>
       <c r="C27" s="41"/>
@@ -9701,7 +10035,7 @@
       <c r="H27" s="33"/>
       <c r="I27" s="33"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
       <c r="B28" s="33"/>
       <c r="C28" s="41"/>
@@ -9712,7 +10046,7 @@
       <c r="H28" s="33"/>
       <c r="I28" s="33"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="33"/>
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
@@ -9723,7 +10057,7 @@
       <c r="H29" s="38"/>
       <c r="I29" s="38"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="33"/>
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
@@ -9734,7 +10068,7 @@
       <c r="H30" s="38"/>
       <c r="I30" s="38"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="33"/>
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
@@ -9745,7 +10079,7 @@
       <c r="H31" s="38"/>
       <c r="I31" s="38"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="33"/>
       <c r="B32" s="33"/>
       <c r="C32" s="41"/>
@@ -10144,6 +10478,242 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20B0DB3-58B5-463D-B8A3-53DC39E150A4}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="15">
+        <v>45120</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="16">
+        <v>96.1</v>
+      </c>
+      <c r="E3" s="16">
+        <v>79</v>
+      </c>
+      <c r="F3" s="16">
+        <v>294.74</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6">
+        <v>45120</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>96</v>
+      </c>
+      <c r="E4" s="4">
+        <v>67.209999999999994</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45120</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>96.6</v>
+      </c>
+      <c r="E5" s="4">
+        <v>61.49</v>
+      </c>
+      <c r="F5" s="4">
+        <v>166.87</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6">
+        <v>45120</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>96.9</v>
+      </c>
+      <c r="E6" s="4">
+        <v>56.77</v>
+      </c>
+      <c r="F6" s="4">
+        <v>93.57</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45127</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>98</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45127</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>98</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45146</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>98</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45146</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>98</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -10152,7 +10722,7 @@
   <dimension ref="A1:L72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding lab IDs to the water samples
</commit_message>
<xml_diff>
--- a/GSD/Water Samples/LaJara_LISST_GSD_Summer2023.xlsx
+++ b/GSD/Water Samples/LaJara_LISST_GSD_Summer2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Water Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1964EDAB-D60A-481C-BFE0-F8216B20E2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A557E42B-2814-40CC-8C66-0FA3195593E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5952B5DA-6B13-43D1-9193-1BE03F62DE4B}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="499">
   <si>
     <t>Dilutions</t>
   </si>
@@ -504,9 +504,6 @@
     <t>SMST237</t>
   </si>
   <si>
-    <t>STORM 2: Aug 28</t>
-  </si>
-  <si>
     <t>SMST238</t>
   </si>
   <si>
@@ -1537,6 +1534,9 @@
   </si>
   <si>
     <t>DOWN 7</t>
+  </si>
+  <si>
+    <t>STORM 3: Aug 28</t>
   </si>
 </sst>
 </file>
@@ -2120,6 +2120,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2138,22 +2153,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2472,7 +2472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68CFA7B-6AB5-4D15-9587-78BC8AED2040}">
   <dimension ref="A1:Q135"/>
   <sheetViews>
-    <sheetView topLeftCell="C99" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P122" sqref="P122"/>
     </sheetView>
   </sheetViews>
@@ -2495,10 +2495,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="70"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -2514,15 +2514,15 @@
       <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="66" t="s">
+      <c r="N2" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="O2" s="67"/>
+      <c r="O2" s="72"/>
       <c r="P2" s="57" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q2" s="31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2551,13 +2551,13 @@
         <v>44</v>
       </c>
       <c r="I3" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="J3" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="J3" s="16" t="s">
-        <v>494</v>
-      </c>
       <c r="K3" s="49" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N3" s="54" t="s">
         <v>44</v>
@@ -2810,13 +2810,13 @@
         <v>74</v>
       </c>
       <c r="I9" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>494</v>
-      </c>
       <c r="K9" s="46" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>63</v>
@@ -3656,7 +3656,7 @@
         <v>54.48</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3679,7 +3679,7 @@
         <v>48.33</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3702,7 +3702,7 @@
         <v>47.29</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3725,7 +3725,7 @@
         <v>52.43</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3748,7 +3748,7 @@
         <v>52.82</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3771,7 +3771,7 @@
         <v>52.94</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3794,7 +3794,7 @@
         <v>46.84</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3817,7 +3817,7 @@
         <v>57.06</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3840,7 +3840,7 @@
         <v>46.39</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3863,7 +3863,7 @@
         <v>47.69</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3886,7 +3886,7 @@
         <v>48.56</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
         <v>33.78</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3932,7 +3932,7 @@
         <v>34.729999999999997</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3955,7 +3955,7 @@
         <v>37.54</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3978,7 +3978,7 @@
         <v>35.24</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -4001,7 +4001,7 @@
         <v>34.76</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -4024,7 +4024,7 @@
         <v>48.15</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -4047,7 +4047,7 @@
         <v>50.42</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -4070,7 +4070,7 @@
         <v>50.96</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -4093,7 +4093,7 @@
         <v>57.76</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -4116,7 +4116,7 @@
         <v>50</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -4139,7 +4139,7 @@
         <v>56.93</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -4162,7 +4162,7 @@
         <v>60.71</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -4185,7 +4185,7 @@
         <v>49.93</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -4208,7 +4208,7 @@
         <v>47.42</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -4231,7 +4231,7 @@
         <v>76.180000000000007</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -4254,7 +4254,7 @@
         <v>80.900000000000006</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -4277,7 +4277,7 @@
         <v>75.09</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -4300,7 +4300,7 @@
         <v>65.23</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -4323,7 +4323,7 @@
         <v>76.97</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -4346,7 +4346,7 @@
         <v>72.17</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -4369,7 +4369,7 @@
         <v>73.53</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -4392,7 +4392,7 @@
         <v>66.12</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -4415,7 +4415,7 @@
         <v>73.08</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -4438,7 +4438,7 @@
         <v>53.75</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>76.03</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -4484,7 +4484,7 @@
         <v>73.95</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -4507,7 +4507,7 @@
         <v>75.400000000000006</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -4530,7 +4530,7 @@
         <v>68.62</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -4553,7 +4553,7 @@
         <v>70.47</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -4691,7 +4691,7 @@
         <v>48.99</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -4714,7 +4714,7 @@
         <v>50.91</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4737,7 +4737,7 @@
         <v>50.39</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4760,7 +4760,7 @@
         <v>47.67</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4783,7 +4783,7 @@
         <v>46.12</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>68.66</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4829,7 +4829,7 @@
         <v>71.33</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,7 @@
         <v>78.010000000000005</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4875,7 +4875,7 @@
         <v>60.5</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4898,7 +4898,7 @@
         <v>56</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4921,7 +4921,7 @@
         <v>58.51</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -4944,7 +4944,7 @@
         <v>63.08</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4967,7 +4967,7 @@
         <v>61.82</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4990,7 +4990,7 @@
         <v>61.69</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -5013,7 +5013,7 @@
         <v>53.82</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -5036,7 +5036,7 @@
         <v>56.87</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -5059,7 +5059,7 @@
         <v>54.2</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -5082,7 +5082,7 @@
         <v>60.2</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
@@ -5105,7 +5105,7 @@
         <v>60.91</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
@@ -5128,7 +5128,7 @@
         <v>64.25</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>54.67</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
@@ -5174,7 +5174,7 @@
         <v>54.54</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
@@ -5197,7 +5197,7 @@
         <v>70.150000000000006</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
@@ -5220,7 +5220,7 @@
         <v>71.55</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
@@ -5243,7 +5243,7 @@
         <v>78</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="104" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5266,7 +5266,7 @@
         <v>61.66</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
@@ -5289,17 +5289,17 @@
         <v>61.69</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="N105" s="68" t="s">
+        <v>190</v>
+      </c>
+      <c r="N105" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="O105" s="69"/>
+      <c r="O105" s="74"/>
       <c r="P105" s="63" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q105" s="31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
@@ -5525,22 +5525,22 @@
         <v>32.47</v>
       </c>
       <c r="G112" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H112" s="60" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I112" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="J112" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="J112" s="1" t="s">
-        <v>494</v>
-      </c>
       <c r="K112" s="46" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L112" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
@@ -5563,7 +5563,7 @@
         <v>45.57</v>
       </c>
       <c r="G113" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H113" s="61">
         <f>K113/(1-($J$113/$I$113))</f>
@@ -5599,7 +5599,7 @@
         <v>32.17</v>
       </c>
       <c r="G114" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H114" s="61">
         <f t="shared" ref="H114:H115" si="1">K114/(1-($J$113/$I$113))</f>
@@ -5631,7 +5631,7 @@
         <v>31.15</v>
       </c>
       <c r="G115" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H115" s="61">
         <f t="shared" si="1"/>
@@ -5663,7 +5663,7 @@
         <v>31.36</v>
       </c>
       <c r="G116" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H116" s="62">
         <f>K116/(1-($J$113/$I$113))</f>
@@ -5695,10 +5695,10 @@
         <v>40.9</v>
       </c>
       <c r="G117" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H117" s="60" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I117" s="1" t="s">
         <v>117</v>
@@ -5707,10 +5707,10 @@
         <v>118</v>
       </c>
       <c r="K117" s="46" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L117" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
@@ -5733,7 +5733,7 @@
         <v>23.42</v>
       </c>
       <c r="G118" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H118" s="61">
         <f>K118/(1-($J$118/$I$118))</f>
@@ -5769,7 +5769,7 @@
         <v>30.13</v>
       </c>
       <c r="G119" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H119" s="61">
         <f t="shared" ref="H119:H122" si="2">K119/(1-($J$118/$I$118))</f>
@@ -5801,7 +5801,7 @@
         <v>31.7</v>
       </c>
       <c r="G120" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H120" s="61">
         <f t="shared" si="2"/>
@@ -5833,7 +5833,7 @@
         <v>29.32</v>
       </c>
       <c r="G121" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H121" s="61">
         <f t="shared" si="2"/>
@@ -5865,7 +5865,7 @@
         <v>28.35</v>
       </c>
       <c r="G122" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H122" s="62">
         <f t="shared" si="2"/>
@@ -5897,7 +5897,7 @@
         <v>44.5</v>
       </c>
       <c r="G123" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
@@ -5920,7 +5920,7 @@
         <v>44.41</v>
       </c>
       <c r="G124" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
@@ -5943,7 +5943,7 @@
         <v>42.41</v>
       </c>
       <c r="G125" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="126" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5966,19 +5966,19 @@
         <v>26.37</v>
       </c>
       <c r="G126" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H126" s="58" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I126" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="J126" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="J126" s="4" t="s">
-        <v>494</v>
-      </c>
       <c r="K126" s="28" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
@@ -6001,7 +6001,7 @@
         <v>49.41</v>
       </c>
       <c r="G127" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H127" s="59">
         <f>K127/(1-($J$127/$I$127))</f>
@@ -6037,7 +6037,7 @@
         <v>51.85</v>
       </c>
       <c r="G128" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -6060,7 +6060,7 @@
         <v>50.11</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -6083,7 +6083,7 @@
         <v>50.53</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -6106,7 +6106,7 @@
         <v>39.94</v>
       </c>
       <c r="G131" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -6129,7 +6129,7 @@
         <v>44.37</v>
       </c>
       <c r="G132" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -6152,7 +6152,7 @@
         <v>45.85</v>
       </c>
       <c r="G133" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -6175,7 +6175,7 @@
         <v>43.16</v>
       </c>
       <c r="G134" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -6198,7 +6198,7 @@
         <v>48.41</v>
       </c>
       <c r="G135" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -6235,10 +6235,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="70"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -6254,15 +6254,15 @@
       <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="65"/>
+      <c r="J2" s="70"/>
       <c r="K2" s="43" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6290,7 +6290,7 @@
       <c r="I3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="71">
+      <c r="J3" s="65">
         <v>45151.78125</v>
       </c>
       <c r="K3" s="1">
@@ -6434,7 +6434,7 @@
       <c r="I7" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="70">
+      <c r="J7" s="64">
         <v>45151.876388888886</v>
       </c>
       <c r="K7" s="48">
@@ -6490,15 +6490,15 @@
       <c r="G9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="72"/>
+      <c r="J9" s="75"/>
       <c r="K9" s="43" t="s">
         <v>2</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -6526,7 +6526,7 @@
       <c r="I10" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="73">
+      <c r="J10" s="66">
         <v>45151.78125</v>
       </c>
       <c r="K10" s="1">
@@ -6922,7 +6922,7 @@
       <c r="I21" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="J21" s="70">
+      <c r="J21" s="64">
         <v>45151.895833333336</v>
       </c>
       <c r="K21" s="48">
@@ -7979,7 +7979,7 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7991,18 +7991,18 @@
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
     <col min="11" max="11" width="22.140625" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="65"/>
+      <c r="A2" s="69" t="s">
+        <v>498</v>
+      </c>
+      <c r="B2" s="70"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -8018,15 +8018,15 @@
       <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="64" t="s">
-        <v>154</v>
-      </c>
-      <c r="J2" s="65"/>
+      <c r="I2" s="69" t="s">
+        <v>498</v>
+      </c>
+      <c r="J2" s="70"/>
       <c r="K2" s="43" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -8047,7 +8047,7 @@
         <v>62.61</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>44</v>
@@ -8079,7 +8079,7 @@
         <v>66.959999999999994</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>74</v>
@@ -8111,7 +8111,7 @@
         <v>65.45</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>50</v>
@@ -8143,7 +8143,7 @@
         <v>67.540000000000006</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>55</v>
@@ -8175,7 +8175,7 @@
         <v>54.59</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>59</v>
@@ -8207,7 +8207,7 @@
         <v>65.86</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>61</v>
@@ -8239,7 +8239,7 @@
         <v>67.790000000000006</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>63</v>
@@ -8271,7 +8271,7 @@
         <v>64.790000000000006</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>65</v>
@@ -8303,7 +8303,7 @@
         <v>66.17</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>67</v>
@@ -8335,7 +8335,7 @@
         <v>66.22</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>83</v>
@@ -8367,7 +8367,7 @@
         <v>52.81</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>89</v>
@@ -8399,7 +8399,7 @@
         <v>53.69</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>94</v>
@@ -8431,7 +8431,7 @@
         <v>55</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>119</v>
@@ -8462,7 +8462,7 @@
         <v>46.56</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -8483,7 +8483,7 @@
         <v>52.54</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -8504,7 +8504,7 @@
         <v>53.22</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -8525,7 +8525,7 @@
         <v>58.67</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -8546,7 +8546,7 @@
         <v>62.73</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -8567,7 +8567,7 @@
         <v>58.29</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -8588,7 +8588,7 @@
         <v>55.57</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -8609,7 +8609,7 @@
         <v>54.48</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -8630,7 +8630,7 @@
         <v>54.39</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -8651,7 +8651,7 @@
         <v>54.47</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -8672,7 +8672,7 @@
         <v>57.35</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -8693,7 +8693,7 @@
         <v>59.32</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -8714,7 +8714,7 @@
         <v>53.16</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -8735,7 +8735,7 @@
         <v>56.07</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -8756,7 +8756,7 @@
         <v>57.69</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -8777,7 +8777,7 @@
         <v>57.34</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -8798,7 +8798,7 @@
         <v>60.09</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -8819,7 +8819,7 @@
         <v>67.540000000000006</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -8840,7 +8840,7 @@
         <v>87.98</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -8861,7 +8861,7 @@
         <v>67.930000000000007</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -8882,7 +8882,7 @@
         <v>66.81</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -8903,7 +8903,7 @@
         <v>67.67</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -8924,7 +8924,7 @@
         <v>55.24</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -8945,7 +8945,7 @@
         <v>57.62</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -8966,7 +8966,7 @@
         <v>54.43</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -8987,7 +8987,7 @@
         <v>54.74</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -9008,7 +9008,7 @@
         <v>55.29</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -9029,7 +9029,7 @@
         <v>54.41</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -9050,7 +9050,7 @@
         <v>51.64</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -9071,7 +9071,7 @@
         <v>50.74</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -9092,7 +9092,7 @@
         <v>54.82</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -9113,7 +9113,7 @@
         <v>53.79</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -9134,7 +9134,7 @@
         <v>52.16</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -9155,7 +9155,7 @@
         <v>47.82</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -9176,7 +9176,7 @@
         <v>49.07</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -9197,7 +9197,7 @@
         <v>47.05</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -9218,7 +9218,7 @@
         <v>47.55</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -9239,7 +9239,7 @@
         <v>56.96</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -9260,7 +9260,7 @@
         <v>60.53</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -9281,7 +9281,7 @@
         <v>71.58</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -9302,7 +9302,7 @@
         <v>60.35</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -9323,7 +9323,7 @@
         <v>76.16</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -9344,7 +9344,7 @@
         <v>67.81</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -9365,7 +9365,7 @@
         <v>75.239999999999995</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -9382,7 +9382,7 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9401,7 +9401,7 @@
   <sheetData>
     <row r="1" spans="1:10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B1" s="34" t="s">
         <v>0</v>
@@ -9410,25 +9410,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" s="35" t="s">
         <v>429</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="35" t="s">
         <v>430</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="G1" s="35" t="s">
+        <v>445</v>
+      </c>
+      <c r="H1" s="35" t="s">
         <v>431</v>
       </c>
-      <c r="G1" s="35" t="s">
-        <v>446</v>
-      </c>
-      <c r="H1" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>432</v>
       </c>
-      <c r="I1" s="35" t="s">
-        <v>433</v>
-      </c>
-      <c r="J1" s="74" t="s">
-        <v>497</v>
+      <c r="J1" s="67" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="2" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
@@ -9452,15 +9452,17 @@
         <v>95.95</v>
       </c>
       <c r="G2" s="25" t="s">
+        <v>448</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>449</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>450</v>
       </c>
-      <c r="I2" s="25" t="s">
-        <v>451</v>
-      </c>
-      <c r="J2" s="44"/>
+      <c r="J2" s="4">
+        <v>490</v>
+      </c>
     </row>
     <row r="3" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -9483,15 +9485,17 @@
         <v>81.680000000000007</v>
       </c>
       <c r="G3" s="25" t="s">
+        <v>451</v>
+      </c>
+      <c r="H3" s="25" t="s">
         <v>452</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="25" t="s">
         <v>453</v>
       </c>
-      <c r="I3" s="25" t="s">
-        <v>454</v>
-      </c>
-      <c r="J3" s="44"/>
+      <c r="J3" s="4">
+        <v>491</v>
+      </c>
     </row>
     <row r="4" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
@@ -9514,15 +9518,17 @@
         <v>71.739999999999995</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>468</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="J4" s="44"/>
+      <c r="J4" s="4">
+        <v>492</v>
+      </c>
     </row>
     <row r="5" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
@@ -9545,15 +9551,17 @@
         <v>48.46</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H5" s="25" t="s">
+        <v>469</v>
+      </c>
+      <c r="I5" s="25" t="s">
         <v>470</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>471</v>
-      </c>
-      <c r="J5" s="44"/>
+      <c r="J5" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
@@ -9576,15 +9584,17 @@
         <v>64.52</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="J6" s="44"/>
+      <c r="J6" s="4">
+        <v>493</v>
+      </c>
     </row>
     <row r="7" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
@@ -9607,15 +9617,17 @@
         <v>48.46</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H7" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="J7" s="44"/>
+      <c r="J7" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="8" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
@@ -9638,15 +9650,17 @@
         <v>60.42</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H8" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="J8" s="44"/>
+      <c r="J8" s="4">
+        <v>494</v>
+      </c>
     </row>
     <row r="9" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
@@ -9669,15 +9683,17 @@
         <v>41.02</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="J9" s="44"/>
+      <c r="J9" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="10" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
@@ -9700,7 +9716,7 @@
         <v>99</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>99</v>
@@ -9708,7 +9724,9 @@
       <c r="I10" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="J10" s="44"/>
+      <c r="J10" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="11" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37"/>
@@ -9724,7 +9742,7 @@
     </row>
     <row r="12" spans="1:10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -9743,13 +9761,13 @@
         <v>64.959999999999994</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H12" s="25" t="s">
+        <v>479</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>480</v>
-      </c>
-      <c r="I12" s="25" t="s">
-        <v>481</v>
       </c>
       <c r="J12" s="4">
         <v>484</v>
@@ -9776,13 +9794,13 @@
         <v>78.52</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H13" s="25" t="s">
+        <v>481</v>
+      </c>
+      <c r="I13" s="25" t="s">
         <v>482</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>483</v>
       </c>
       <c r="J13" s="4">
         <v>485</v>
@@ -9809,13 +9827,13 @@
         <v>72.900000000000006</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H14" s="25" t="s">
+        <v>483</v>
+      </c>
+      <c r="I14" s="25" t="s">
         <v>484</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>485</v>
       </c>
       <c r="J14" s="4">
         <v>486</v>
@@ -9842,13 +9860,13 @@
         <v>61.13</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H15" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>486</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>487</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>99</v>
@@ -9875,13 +9893,13 @@
         <v>85.72</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H16" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>488</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>489</v>
       </c>
       <c r="J16" s="4">
         <v>487</v>
@@ -9908,13 +9926,13 @@
         <v>55.4</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H17" s="25" t="s">
+        <v>489</v>
+      </c>
+      <c r="I17" s="25" t="s">
         <v>490</v>
-      </c>
-      <c r="I17" s="25" t="s">
-        <v>491</v>
       </c>
       <c r="J17" s="4">
         <v>488</v>
@@ -9922,10 +9940,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B18" s="32"/>
-      <c r="C18" s="75"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
@@ -10487,7 +10505,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10502,10 +10520,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="65"/>
+      <c r="B2" s="70"/>
       <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
@@ -10739,7 +10757,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -10748,27 +10766,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="24" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>429</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>430</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" s="24" t="s">
+        <v>445</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>431</v>
       </c>
-      <c r="G1" s="24" t="s">
-        <v>446</v>
-      </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>432</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -10795,15 +10813,15 @@
         <v>99</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -10830,7 +10848,7 @@
         <v>99</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L3" s="4">
         <v>300</v>
@@ -10838,7 +10856,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -10857,16 +10875,16 @@
         <v>24.4</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>436</v>
-      </c>
       <c r="K4" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L4" s="4">
         <v>200</v>
@@ -10874,7 +10892,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -10903,7 +10921,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -10922,24 +10940,24 @@
         <v>99</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>438</v>
-      </c>
       <c r="I6" s="4" t="s">
         <v>99</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L6" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -10960,16 +10978,16 @@
         <v>99</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>443</v>
-      </c>
       <c r="I7" s="4" t="s">
         <v>99</v>
       </c>
       <c r="K7" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L7" s="4">
         <v>500</v>
@@ -10977,7 +10995,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -10999,16 +11017,16 @@
         <v>256.68333333333334</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>445</v>
-      </c>
       <c r="I8" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K8" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L8" s="4">
         <v>200</v>
@@ -11016,7 +11034,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -11035,18 +11053,18 @@
         <v>146.46</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>319</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
@@ -11073,15 +11091,15 @@
         <v>99</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L10" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B11" s="4">
         <v>0</v>
@@ -11108,7 +11126,7 @@
         <v>99</v>
       </c>
       <c r="K11" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L11" s="4">
         <v>300</v>
@@ -11116,7 +11134,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -11143,7 +11161,7 @@
         <v>99</v>
       </c>
       <c r="K12" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L12" s="4">
         <v>200</v>
@@ -11151,7 +11169,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -11180,7 +11198,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B14" s="4">
         <v>0</v>
@@ -11207,15 +11225,15 @@
         <v>99</v>
       </c>
       <c r="K14" s="29" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
@@ -11236,16 +11254,16 @@
         <v>99</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>323</v>
-      </c>
       <c r="I15" s="4" t="s">
         <v>99</v>
       </c>
       <c r="K15" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L15" s="4">
         <v>200</v>
@@ -11253,7 +11271,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -11275,16 +11293,16 @@
         <v>463.82</v>
       </c>
       <c r="G16" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>326</v>
-      </c>
       <c r="K16" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L16" s="4">
         <v>100</v>
@@ -11292,7 +11310,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -11321,7 +11339,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -11343,24 +11361,24 @@
         <v>278.58</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="I18" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>329</v>
-      </c>
       <c r="K18" s="29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L18" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
@@ -11387,7 +11405,7 @@
         <v>99</v>
       </c>
       <c r="K19" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L19" s="4">
         <v>400</v>
@@ -11395,7 +11413,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B20" s="4">
         <v>0</v>
@@ -11422,7 +11440,7 @@
         <v>99</v>
       </c>
       <c r="K20" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L20" s="4">
         <v>200</v>
@@ -11430,7 +11448,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B21" s="4">
         <v>0</v>
@@ -11459,42 +11477,42 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+      <c r="C22" s="18">
+        <v>0</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="K22" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="B22" s="4">
-        <v>0</v>
-      </c>
-      <c r="C22" s="18">
-        <v>0</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" s="29" t="s">
-        <v>333</v>
-      </c>
       <c r="L22" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
@@ -11516,16 +11534,16 @@
         <v>367.27499999999998</v>
       </c>
       <c r="G23" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>332</v>
-      </c>
       <c r="K23" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L23" s="4">
         <v>500</v>
@@ -11533,7 +11551,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -11555,16 +11573,16 @@
         <v>275.97499999999997</v>
       </c>
       <c r="G24" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="I24" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>335</v>
-      </c>
       <c r="K24" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L24" s="4">
         <v>300</v>
@@ -11572,7 +11590,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
@@ -11594,18 +11612,18 @@
         <v>139.48333333333335</v>
       </c>
       <c r="G25" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="I25" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
@@ -11627,24 +11645,24 @@
         <v>136.44999999999999</v>
       </c>
       <c r="G26" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>341</v>
-      </c>
       <c r="K26" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L26" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B27" s="4">
         <v>0</v>
@@ -11663,16 +11681,16 @@
         <v>82.57</v>
       </c>
       <c r="G27" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>344</v>
-      </c>
       <c r="K27" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L27" s="4">
         <v>500</v>
@@ -11680,7 +11698,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B28" s="4">
         <v>0</v>
@@ -11699,16 +11717,16 @@
         <v>79.47</v>
       </c>
       <c r="G28" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="I28" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>347</v>
-      </c>
       <c r="K28" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L28" s="4">
         <v>300</v>
@@ -11716,7 +11734,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B29" s="4">
         <v>0</v>
@@ -11745,7 +11763,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B30" s="4">
         <v>0</v>
@@ -11772,15 +11790,15 @@
         <v>99</v>
       </c>
       <c r="K30" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L30" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B31" s="4">
         <v>0</v>
@@ -11807,7 +11825,7 @@
         <v>99</v>
       </c>
       <c r="K31" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L31" s="4">
         <v>500</v>
@@ -11815,7 +11833,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B32" s="4">
         <v>0</v>
@@ -11834,16 +11852,16 @@
         <v>204.33</v>
       </c>
       <c r="G32" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="I32" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="I32" s="4" t="s">
-        <v>350</v>
-      </c>
       <c r="K32" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L32" s="4">
         <v>200</v>
@@ -11851,7 +11869,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
@@ -11873,18 +11891,18 @@
         <v>373.66</v>
       </c>
       <c r="G33" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="H33" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>358</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B34" s="4">
         <v>0</v>
@@ -11903,24 +11921,24 @@
         <v>219.5</v>
       </c>
       <c r="G34" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="I34" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="I34" s="4" t="s">
-        <v>353</v>
-      </c>
       <c r="K34" s="29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L34" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
@@ -11939,16 +11957,16 @@
         <v>190.38</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="I35" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="I35" s="4" t="s">
-        <v>356</v>
-      </c>
       <c r="K35" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L35" s="4">
         <v>500</v>
@@ -11956,7 +11974,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B36" s="4">
         <v>0</v>
@@ -11975,16 +11993,16 @@
         <v>103.1</v>
       </c>
       <c r="G36" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="I36" s="4" t="s">
-        <v>362</v>
-      </c>
       <c r="K36" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L36" s="4">
         <v>100</v>
@@ -11992,7 +12010,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B37" s="4">
         <v>0</v>
@@ -12011,18 +12029,18 @@
         <v>91.84</v>
       </c>
       <c r="G37" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="I37" s="4" t="s">
         <v>364</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B38" s="4">
         <v>0</v>
@@ -12041,24 +12059,24 @@
         <v>32.14</v>
       </c>
       <c r="G38" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="H38" s="4" t="s">
         <v>366</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="I38" s="4" t="s">
-        <v>368</v>
-      </c>
       <c r="K38" s="29" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B39" s="4">
         <v>0</v>
@@ -12085,7 +12103,7 @@
         <v>99</v>
       </c>
       <c r="K39" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L39" s="4">
         <v>400</v>
@@ -12093,7 +12111,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B40" s="4">
         <v>0</v>
@@ -12112,16 +12130,16 @@
         <v>40.69</v>
       </c>
       <c r="G40" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="H40" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="I40" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="I40" s="4" t="s">
-        <v>395</v>
-      </c>
       <c r="K40" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L40" s="4">
         <v>200</v>
@@ -12129,7 +12147,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B41" s="4">
         <v>0</v>
@@ -12158,42 +12176,42 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0</v>
+      </c>
+      <c r="C42" s="18">
+        <v>0</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="I42" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="K42" s="29" t="s">
         <v>357</v>
       </c>
-      <c r="B42" s="4">
-        <v>0</v>
-      </c>
-      <c r="C42" s="18">
-        <v>0</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F42" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="G42" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="H42" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="I42" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="K42" s="29" t="s">
-        <v>358</v>
-      </c>
       <c r="L42" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
@@ -12215,16 +12233,16 @@
         <v>845.92</v>
       </c>
       <c r="G43" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="I43" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="I43" s="4" t="s">
-        <v>398</v>
-      </c>
       <c r="K43" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L43" s="4">
         <v>400</v>
@@ -12232,7 +12250,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B44" s="4">
         <v>0</v>
@@ -12251,16 +12269,16 @@
         <v>121.08</v>
       </c>
       <c r="G44" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="H44" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="H44" s="4" t="s">
+      <c r="I44" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>401</v>
-      </c>
       <c r="K44" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L44" s="4">
         <v>300</v>
@@ -12268,7 +12286,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
@@ -12290,18 +12308,18 @@
         <v>631.04</v>
       </c>
       <c r="G45" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="H45" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="H45" s="4" t="s">
+      <c r="I45" s="4" t="s">
         <v>403</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
@@ -12323,24 +12341,24 @@
         <v>915.04</v>
       </c>
       <c r="G46" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="H46" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="I46" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>407</v>
-      </c>
       <c r="K46" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L46" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
@@ -12362,16 +12380,16 @@
         <v>578.29999999999995</v>
       </c>
       <c r="G47" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="H47" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="I47" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="I47" s="4" t="s">
-        <v>410</v>
-      </c>
       <c r="K47" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L47" s="4">
         <v>400</v>
@@ -12379,7 +12397,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
@@ -12401,16 +12419,16 @@
         <v>578.29999999999995</v>
       </c>
       <c r="G48" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="H48" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="I48" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="I48" s="4" t="s">
-        <v>413</v>
-      </c>
       <c r="K48" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L48" s="4">
         <v>300</v>
@@ -12418,7 +12436,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B49" s="4">
         <v>0</v>
@@ -12440,18 +12458,18 @@
         <v>122.95</v>
       </c>
       <c r="G49" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="H49" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="I49" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B50" s="4">
         <v>0</v>
@@ -12478,15 +12496,15 @@
         <v>99</v>
       </c>
       <c r="K50" s="29" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L50" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B51" s="4">
         <v>0</v>
@@ -12513,7 +12531,7 @@
         <v>99</v>
       </c>
       <c r="K51" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L51" s="4">
         <v>400</v>
@@ -12521,7 +12539,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B52" s="4">
         <v>0</v>
@@ -12548,7 +12566,7 @@
         <v>99</v>
       </c>
       <c r="K52" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L52" s="4">
         <v>300</v>
@@ -12556,7 +12574,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
@@ -12578,18 +12596,18 @@
         <v>491.26</v>
       </c>
       <c r="G53" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="H53" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="H53" s="4" t="s">
+      <c r="I53" s="4" t="s">
         <v>418</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
@@ -12611,24 +12629,24 @@
         <v>308.16666666666669</v>
       </c>
       <c r="G54" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="H54" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="H54" s="4" t="s">
+      <c r="I54" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="I54" s="4" t="s">
-        <v>422</v>
-      </c>
       <c r="K54" s="29" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L54" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B55" s="4">
         <v>0</v>
@@ -12647,16 +12665,16 @@
         <v>242.57</v>
       </c>
       <c r="G55" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="H55" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="H55" s="4" t="s">
+      <c r="I55" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="I55" s="4" t="s">
-        <v>425</v>
-      </c>
       <c r="K55" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L55" s="4">
         <v>400</v>
@@ -12664,7 +12682,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B56" s="4">
         <v>0</v>
@@ -12683,16 +12701,16 @@
         <v>191.22</v>
       </c>
       <c r="G56" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="H56" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="H56" s="4" t="s">
+      <c r="I56" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="I56" s="4" t="s">
-        <v>428</v>
-      </c>
       <c r="K56" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L56" s="4">
         <v>200</v>
@@ -12700,7 +12718,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B57" s="4">
         <v>0</v>
@@ -12719,18 +12737,18 @@
         <v>132.82</v>
       </c>
       <c r="G57" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="H57" s="4" t="s">
+      <c r="I57" s="4" t="s">
         <v>370</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B58" s="4">
         <v>0</v>
@@ -12749,24 +12767,24 @@
         <v>103.48</v>
       </c>
       <c r="G58" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="H58" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="H58" s="4" t="s">
+      <c r="I58" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="I58" s="4" t="s">
-        <v>374</v>
-      </c>
       <c r="K58" s="29" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L58" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B59" s="4">
         <v>0</v>
@@ -12793,7 +12811,7 @@
         <v>99</v>
       </c>
       <c r="K59" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L59" s="4">
         <v>400</v>
@@ -12801,7 +12819,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B60" s="4">
         <v>0</v>
@@ -12828,7 +12846,7 @@
         <v>99</v>
       </c>
       <c r="K60" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L60" s="4">
         <v>200</v>
@@ -12836,7 +12854,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B61" s="4">
         <v>0</v>
@@ -12865,7 +12883,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B62" s="4">
         <v>1</v>
@@ -12887,24 +12905,24 @@
         <v>327.82</v>
       </c>
       <c r="G62" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="H62" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="H62" s="4" t="s">
+      <c r="I62" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="I62" s="4" t="s">
-        <v>377</v>
-      </c>
       <c r="K62" s="29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L62" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B63" s="4">
         <v>0</v>
@@ -12923,16 +12941,16 @@
         <v>228.79</v>
       </c>
       <c r="G63" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="H63" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="H63" s="4" t="s">
+      <c r="I63" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="I63" s="4" t="s">
-        <v>383</v>
-      </c>
       <c r="K63" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L63" s="4">
         <v>400</v>
@@ -12940,7 +12958,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B64" s="4">
         <v>0</v>
@@ -12959,16 +12977,16 @@
         <v>207.15</v>
       </c>
       <c r="G64" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="H64" s="4" t="s">
         <v>378</v>
       </c>
-      <c r="H64" s="4" t="s">
+      <c r="I64" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="I64" s="4" t="s">
-        <v>380</v>
-      </c>
       <c r="K64" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L64" s="4">
         <v>200</v>
@@ -12976,7 +12994,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B65" s="4">
         <v>0</v>
@@ -12995,18 +13013,18 @@
         <v>133.51</v>
       </c>
       <c r="G65" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="H65" s="25" t="s">
         <v>384</v>
       </c>
-      <c r="H65" s="25" t="s">
+      <c r="I65" s="25" t="s">
         <v>385</v>
-      </c>
-      <c r="I65" s="25" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B66" s="4">
         <v>0</v>
@@ -13025,24 +13043,24 @@
         <v>88.41</v>
       </c>
       <c r="G66" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="H66" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="H66" s="4" t="s">
+      <c r="I66" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="I66" s="4" t="s">
-        <v>389</v>
-      </c>
       <c r="K66" s="29" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L66" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B67" s="4">
         <v>0</v>
@@ -13061,16 +13079,16 @@
         <v>60.39</v>
       </c>
       <c r="G67" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="H67" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="H67" s="4" t="s">
+      <c r="I67" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="I67" s="4" t="s">
-        <v>392</v>
-      </c>
       <c r="K67" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L67" s="4">
         <v>500</v>
@@ -13078,7 +13096,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K68" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L68" s="4">
         <v>200</v>
@@ -13086,15 +13104,15 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K70" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L70" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K71" s="28" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L71" s="4">
         <v>400</v>
@@ -13102,7 +13120,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K72" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L72" s="4">
         <v>200</v>

</xml_diff>

<commit_message>
update on hysteresis code and csv :)
</commit_message>
<xml_diff>
--- a/GSD/Water Samples/LaJara_LISST_GSD_Summer2023.xlsx
+++ b/GSD/Water Samples/LaJara_LISST_GSD_Summer2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Water Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A557E42B-2814-40CC-8C66-0FA3195593E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA8C1F9-FFD2-4E9F-9E1B-7167DD19A950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5952B5DA-6B13-43D1-9193-1BE03F62DE4B}"/>
   </bookViews>
@@ -1548,7 +1548,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1575,6 +1575,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1937,7 +1944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2154,6 +2161,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7979,7 +7992,7 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9382,7 +9395,7 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9637,16 +9650,16 @@
         <v>0</v>
       </c>
       <c r="C8" s="27">
-        <f t="shared" si="0"/>
-        <v>52.79999999999999</v>
+        <f>AVERAGE(D8)</f>
+        <v>46.07</v>
       </c>
       <c r="D8" s="4">
         <v>46.07</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="76">
         <v>51.91</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="77">
         <v>60.42</v>
       </c>
       <c r="G8" s="4" t="s">

</xml_diff>